<commit_message>
Name corrections + Added QBP and prompt examples
</commit_message>
<xml_diff>
--- a/similarity_matrix.xlsx
+++ b/similarity_matrix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC25"/>
+  <dimension ref="A1:AG25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,136 +446,156 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>activity1 (Rapid initial evaluation for airway, breathing, and circulation)</t>
+          <t>activity1-1 (Rapid initial evaluation for airway, breathing, and circulation)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>activity1-2 (Rapid initial evaluation for airway, breathing, and circulation)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>activity1-3 (Rapid initial evaluation for airway, breathing, and circulation)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>parallelgateway1 (Parallel Gateway)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>dummy_Flow_2 ((dummy branch entry))</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>activity2 (Immediate brain imaging (CT or MRI))</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>activity3 (Immediate brain imaging (CT or MRI))</t>
+          <t>activity2 (neurological examination to determine focal neurological deficits and assess stroke severity on a standardized stroke scale (NIHSS or CNS for stroke))</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>dummy_Flow_4 ((dummy branch entry))</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>activity3-1 (Immediate brain imaging (CT or MRI))</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>activity3-2 (Immediate brain imaging (CT or MRI))</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>activity4 (Immediate expert healthcare provider interpretation of the brain imaging)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>activity5 (neurological examination to determine focal neurological deficits and assess stroke severity on a standardized stroke scale (NIHSS or CNS for stroke))</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>activity6 (ECG to detect atrial fibrillation and other acute arrhythmias)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>dummy_Flow_6 ((dummy branch entry))</t>
-        </is>
-      </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>activity7 (Blood work:
+          <t>activity4-1 (Chest x-ray without delay for for thrombolysis assessment)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>activity5 (ECG to detect atrial fibrillation and other acute arrhythmias)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>dummy_Flow_9 ((dummy branch entry))</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>activity6-1 (Blood work:
  CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>activity8 (Blood work:
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>activity6-2 (Blood work:
  CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>activity9 (Chest x-ray without delay for for thrombolysis assessment)</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>dummy_Flow_9 ((dummy branch entry))</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>activity10 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
-        </is>
-      </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>activity11 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
+          <t>parallelgateway1Join (Parallel Merge)</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
+          <t>activity8 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>exclusivegateway1 (Exclusive Gateway)</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>activity12 (Monitor patient closely and swallowing ability screened when clinically appropriate)</t>
-        </is>
-      </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>activity13 (Full clinical assessment of the patient's swallowing ability by an expert (by a speech-language pathologist or appropriately trained specialist who would advise on swallowing ability and the required consistency of diet and fluids))</t>
+          <t>activity9 (Monitor patient closely and swallowing ability screened when clinically appropriate)</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
+          <t>activity10 (Proceed with further assessment as indicated (Role: medical staff; Objects: patient))</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
           <t>exclusivegateway1Join (Exclusive Merge)</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>activity14 (Give patients appropriate cross-continuum secondary prevention assessments and therapies
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>exclusivegateway2 (Exclusive Gateway)</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>activity11 (Full clinical assessment of the patient's swallowing ability by an expert (by a speech-language pathologist or appropriately trained specialist who would advise on swallowing ability and the required consistency of diet and fluids))</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>activity12 (Continue standard care (Role: medical staff; Objects: patient))</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>exclusivegateway2Join (Exclusive Merge)</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>activity13 (Give patients appropriate cross-continuum secondary prevention assessments and therapies
 (All patients, whether admitted or discharged from the ED)</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>activity15 (Use a standard triage tool to determine the appropriate location for the care of patients
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>activity14 (Use a standard triage tool to determine the appropriate location for the care of patients
 (Patients with TIA))</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>exclusivegateway2 (Exclusive Gateway)</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>activity16 (Immediate vascular imaging of the neck arteries (carotid ultrasound, CTA, or MRA))</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>activity17 (Vascular imaging of the brain and neck arteries ASAP)</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>exclusivegateway2Join (Exclusive Merge)</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>parallelgateway1Join (Parallel Merge)</t>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>exclusivegateway3 (Exclusive Gateway)</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>activity15 (Immediate vascular imaging of the neck arteries (carotid ultrasound, CTA, or MRA))</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>activity16 (Vascular imaging of the brain and neck arteries ASAP)</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>exclusivegateway3Join (Exclusive Merge)</t>
         </is>
       </c>
     </row>
@@ -669,6 +689,18 @@
       <c r="AC2" t="n">
         <v>0</v>
       </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -686,78 +718,90 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.214765100671141</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.1746031746031746</v>
       </c>
-      <c r="G3" t="n">
+      <c r="J3" t="n">
         <v>0.253968253968254</v>
       </c>
-      <c r="H3" t="n">
+      <c r="K3" t="n">
         <v>0.253968253968254</v>
       </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
         <v>0.2361111111111112</v>
       </c>
-      <c r="J3" t="n">
-        <v>0.214765100671141</v>
-      </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>0.1746031746031746</v>
       </c>
-      <c r="L3" t="n">
+      <c r="N3" t="n">
         <v>0.1746031746031746</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.2307692307692307</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.2307692307692307</v>
       </c>
       <c r="O3" t="n">
         <v>0.1746031746031746</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1746031746031746</v>
+        <v>0.2307692307692307</v>
       </c>
       <c r="Q3" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
         <v>0.2209302325581395</v>
       </c>
-      <c r="R3" t="n">
-        <v>0.2209302325581395</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
       <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
         <v>0.2409638554216867</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
+        <v>0.2261904761904762</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
         <v>0.1861471861471862</v>
       </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="n">
+      <c r="Z3" t="n">
+        <v>0.1587301587301587</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
         <v>0.1986301369863014</v>
       </c>
-      <c r="X3" t="n">
+      <c r="AC3" t="n">
         <v>0.2477064220183486</v>
       </c>
-      <c r="Y3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="n">
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
         <v>0.1975308641975309</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AF3" t="n">
         <v>0.2380952380952381</v>
       </c>
-      <c r="AB3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC3" t="n">
+      <c r="AG3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -777,78 +821,90 @@
         <v>0.214765100671141</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.214765100671141</v>
       </c>
       <c r="F4" t="n">
+        <v>0.214765100671141</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.09395973154362414</v>
       </c>
-      <c r="G4" t="n">
+      <c r="J4" t="n">
         <v>0.1476510067114094</v>
       </c>
-      <c r="H4" t="n">
+      <c r="K4" t="n">
         <v>0.1476510067114094</v>
       </c>
-      <c r="I4" t="n">
+      <c r="L4" t="n">
         <v>0.2080536912751678</v>
       </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
+        <v>0.1879194630872483</v>
+      </c>
+      <c r="N4" t="n">
         <v>0.2348993288590604</v>
       </c>
-      <c r="L4" t="n">
+      <c r="O4" t="n">
         <v>0.09395973154362414</v>
       </c>
-      <c r="M4" t="n">
+      <c r="P4" t="n">
         <v>0.174496644295302</v>
       </c>
-      <c r="N4" t="n">
+      <c r="Q4" t="n">
         <v>0.174496644295302</v>
       </c>
-      <c r="O4" t="n">
-        <v>0.1879194630872483</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.09395973154362414</v>
-      </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
         <v>0.2325581395348837</v>
       </c>
-      <c r="R4" t="n">
-        <v>0.2325581395348837</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
       <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
         <v>0.2416107382550335</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
+        <v>0.2281879194630873</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
         <v>0.2683982683982684</v>
       </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="n">
+      <c r="Z4" t="n">
+        <v>0.1946308724832215</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="n">
         <v>0.174496644295302</v>
       </c>
-      <c r="X4" t="n">
+      <c r="AC4" t="n">
         <v>0.2885906040268457</v>
       </c>
-      <c r="Y4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="n">
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
         <v>0.2348993288590604</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AF4" t="n">
         <v>0.2013422818791947</v>
       </c>
-      <c r="AB4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC4" t="n">
+      <c r="AG4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -868,78 +924,90 @@
         <v>0.253968253968254</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.253968253968254</v>
       </c>
       <c r="F5" t="n">
+        <v>0.253968253968254</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.1476510067114094</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.2571428571428571</v>
       </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
         <v>0.3055555555555556</v>
       </c>
-      <c r="J5" t="n">
-        <v>0.1476510067114094</v>
-      </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
+        <v>0.1403508771929824</v>
+      </c>
+      <c r="N5" t="n">
         <v>0.2295081967213115</v>
       </c>
-      <c r="L5" t="n">
+      <c r="O5" t="n">
         <v>0.2571428571428571</v>
       </c>
-      <c r="M5" t="n">
+      <c r="P5" t="n">
         <v>0.1538461538461539</v>
       </c>
-      <c r="N5" t="n">
+      <c r="Q5" t="n">
         <v>0.1538461538461539</v>
       </c>
-      <c r="O5" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.2571428571428571</v>
-      </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
         <v>0.1279069767441861</v>
       </c>
-      <c r="R5" t="n">
-        <v>0.1279069767441861</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
       <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
         <v>0.1686746987951807</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
+        <v>0.1904761904761905</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
         <v>0.09956709956709953</v>
       </c>
-      <c r="V5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W5" t="n">
+      <c r="Z5" t="n">
+        <v>0.1774193548387096</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
         <v>0.136986301369863</v>
       </c>
-      <c r="X5" t="n">
+      <c r="AC5" t="n">
         <v>0.1743119266055045</v>
       </c>
-      <c r="Y5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="n">
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
         <v>0.3580246913580247</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AF5" t="n">
         <v>0.25</v>
       </c>
-      <c r="AB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="n">
+      <c r="AG5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -959,78 +1027,90 @@
         <v>0.2361111111111112</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.2361111111111112</v>
       </c>
       <c r="F6" t="n">
+        <v>0.2361111111111112</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.2080536912751678</v>
+      </c>
+      <c r="I6" t="n">
         <v>0.1388888888888888</v>
       </c>
-      <c r="G6" t="n">
+      <c r="J6" t="n">
         <v>0.3055555555555556</v>
       </c>
-      <c r="H6" t="n">
+      <c r="K6" t="n">
         <v>0.3055555555555556</v>
       </c>
-      <c r="I6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.2080536912751678</v>
-      </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="N6" t="n">
         <v>0.2638888888888888</v>
       </c>
-      <c r="L6" t="n">
+      <c r="O6" t="n">
         <v>0.1388888888888888</v>
       </c>
-      <c r="M6" t="n">
+      <c r="P6" t="n">
         <v>0.2307692307692307</v>
       </c>
-      <c r="N6" t="n">
+      <c r="Q6" t="n">
         <v>0.2307692307692307</v>
       </c>
-      <c r="O6" t="n">
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.2209302325581395</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.1807228915662651</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.2142857142857143</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.2034632034632035</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.273972602739726</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.3027522935779816</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0.2592592592592593</v>
+      </c>
+      <c r="AF6" t="n">
         <v>0.2222222222222222</v>
       </c>
-      <c r="P6" t="n">
-        <v>0.1388888888888888</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.2209302325581395</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.2209302325581395</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.1807228915662651</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.2034632034632035</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0.273972602739726</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0.3027522935779816</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0.2592592592592593</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" t="n">
+      <c r="AG6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1050,78 +1130,90 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.1746031746031746</v>
       </c>
       <c r="F7" t="n">
+        <v>0.1746031746031746</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.2348993288590604</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.180327868852459</v>
       </c>
-      <c r="G7" t="n">
+      <c r="J7" t="n">
         <v>0.2295081967213115</v>
       </c>
-      <c r="H7" t="n">
+      <c r="K7" t="n">
         <v>0.2295081967213115</v>
       </c>
-      <c r="I7" t="n">
+      <c r="L7" t="n">
         <v>0.2638888888888888</v>
       </c>
-      <c r="J7" t="n">
-        <v>0.2348993288590604</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>0.180327868852459</v>
       </c>
-      <c r="M7" t="n">
-        <v>0.2384615384615385</v>
-      </c>
       <c r="N7" t="n">
-        <v>0.2384615384615385</v>
+        <v>1</v>
       </c>
       <c r="O7" t="n">
         <v>0.180327868852459</v>
       </c>
       <c r="P7" t="n">
-        <v>0.180327868852459</v>
+        <v>0.2384615384615385</v>
       </c>
       <c r="Q7" t="n">
+        <v>0.2384615384615385</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
         <v>0.1976744186046512</v>
       </c>
-      <c r="R7" t="n">
-        <v>0.1976744186046512</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0</v>
-      </c>
       <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
         <v>0.2771084337349398</v>
       </c>
-      <c r="U7" t="n">
+      <c r="V7" t="n">
+        <v>0.2023809523809523</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
         <v>0.1688311688311688</v>
       </c>
-      <c r="V7" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" t="n">
+      <c r="Z7" t="n">
+        <v>0.1451612903225806</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="n">
         <v>0.2397260273972602</v>
       </c>
-      <c r="X7" t="n">
+      <c r="AC7" t="n">
         <v>0.2752293577981652</v>
       </c>
-      <c r="Y7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z7" t="n">
+      <c r="AD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="n">
         <v>0.1975308641975309</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AF7" t="n">
         <v>0.2459016393442623</v>
       </c>
-      <c r="AB7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC7" t="n">
+      <c r="AG7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1141,78 +1233,90 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.1746031746031746</v>
       </c>
       <c r="F8" t="n">
+        <v>0.1746031746031746</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.1879194630872483</v>
+      </c>
+      <c r="I8" t="n">
         <v>0.1403508771929824</v>
       </c>
-      <c r="G8" t="n">
+      <c r="J8" t="n">
         <v>0.1403508771929824</v>
       </c>
-      <c r="H8" t="n">
+      <c r="K8" t="n">
         <v>0.1403508771929824</v>
       </c>
-      <c r="I8" t="n">
+      <c r="L8" t="n">
         <v>0.2222222222222222</v>
       </c>
-      <c r="J8" t="n">
-        <v>0.1879194630872483</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
         <v>0.180327868852459</v>
       </c>
-      <c r="L8" t="n">
+      <c r="O8" t="n">
         <v>0.1403508771929824</v>
       </c>
-      <c r="M8" t="n">
+      <c r="P8" t="n">
         <v>0.2230769230769231</v>
       </c>
-      <c r="N8" t="n">
+      <c r="Q8" t="n">
         <v>0.2230769230769231</v>
       </c>
-      <c r="O8" t="n">
-        <v>1</v>
-      </c>
-      <c r="P8" t="n">
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.2034883720930233</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.2168674698795181</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.2023809523809523</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.1558441558441559</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.1612903225806451</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.1917808219178082</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.2568807339449541</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0.1975308641975309</v>
+      </c>
+      <c r="AF8" t="n">
         <v>0.1403508771929824</v>
       </c>
-      <c r="Q8" t="n">
-        <v>0.2034883720930233</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.2034883720930233</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" t="n">
-        <v>0.2168674698795181</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0.1558441558441559</v>
-      </c>
-      <c r="V8" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" t="n">
-        <v>0.1917808219178082</v>
-      </c>
-      <c r="X8" t="n">
-        <v>0.2568807339449541</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>0.1975308641975309</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" t="n">
+      <c r="AG8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1233,78 +1337,90 @@
         <v>0.2307692307692307</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.2307692307692307</v>
       </c>
       <c r="F9" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.174496644295302</v>
+      </c>
+      <c r="I9" t="n">
         <v>0.1153846153846154</v>
       </c>
-      <c r="G9" t="n">
+      <c r="J9" t="n">
         <v>0.1538461538461539</v>
       </c>
-      <c r="H9" t="n">
+      <c r="K9" t="n">
         <v>0.1538461538461539</v>
       </c>
-      <c r="I9" t="n">
+      <c r="L9" t="n">
         <v>0.2307692307692307</v>
       </c>
-      <c r="J9" t="n">
-        <v>0.174496644295302</v>
-      </c>
-      <c r="K9" t="n">
+      <c r="M9" t="n">
+        <v>0.2230769230769231</v>
+      </c>
+      <c r="N9" t="n">
         <v>0.2384615384615385</v>
       </c>
-      <c r="L9" t="n">
+      <c r="O9" t="n">
         <v>0.1153846153846154</v>
       </c>
-      <c r="M9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.2441860465116279</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.2769230769230769</v>
+      </c>
+      <c r="V9" t="n">
         <v>0.2230769230769231</v>
       </c>
-      <c r="P9" t="n">
-        <v>0.1153846153846154</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.2441860465116279</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0.2441860465116279</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0.2769230769230769</v>
-      </c>
-      <c r="U9" t="n">
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
         <v>0.2251082251082251</v>
-      </c>
-      <c r="V9" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0.178082191780822</v>
-      </c>
-      <c r="X9" t="n">
-        <v>0.2461538461538462</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>0</v>
       </c>
       <c r="Z9" t="n">
         <v>0.2076923076923077</v>
       </c>
       <c r="AA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.178082191780822</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.2461538461538462</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0.2076923076923077</v>
+      </c>
+      <c r="AF9" t="n">
         <v>0.1923076923076923</v>
       </c>
-      <c r="AB9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC9" t="n">
+      <c r="AG9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1324,78 +1440,90 @@
         <v>0.2209302325581395</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.2209302325581395</v>
       </c>
       <c r="F10" t="n">
+        <v>0.2209302325581395</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.2325581395348837</v>
+      </c>
+      <c r="I10" t="n">
         <v>0.07558139534883723</v>
       </c>
-      <c r="G10" t="n">
+      <c r="J10" t="n">
         <v>0.1279069767441861</v>
       </c>
-      <c r="H10" t="n">
+      <c r="K10" t="n">
         <v>0.1279069767441861</v>
       </c>
-      <c r="I10" t="n">
+      <c r="L10" t="n">
         <v>0.2209302325581395</v>
       </c>
-      <c r="J10" t="n">
-        <v>0.2325581395348837</v>
-      </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
+        <v>0.2034883720930233</v>
+      </c>
+      <c r="N10" t="n">
         <v>0.1976744186046512</v>
       </c>
-      <c r="L10" t="n">
+      <c r="O10" t="n">
         <v>0.07558139534883723</v>
       </c>
-      <c r="M10" t="n">
+      <c r="P10" t="n">
         <v>0.2441860465116279</v>
       </c>
-      <c r="N10" t="n">
+      <c r="Q10" t="n">
         <v>0.2441860465116279</v>
       </c>
-      <c r="O10" t="n">
-        <v>0.2034883720930233</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.07558139534883723</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>1</v>
-      </c>
       <c r="R10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
         <v>0.2906976744186046</v>
       </c>
-      <c r="U10" t="n">
+      <c r="V10" t="n">
+        <v>0.2209302325581395</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
         <v>0.2727272727272727</v>
       </c>
-      <c r="V10" t="n">
-        <v>0</v>
-      </c>
-      <c r="W10" t="n">
+      <c r="Z10" t="n">
+        <v>0.1918604651162791</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="n">
         <v>0.2674418604651163</v>
       </c>
-      <c r="X10" t="n">
+      <c r="AC10" t="n">
         <v>0.2558139534883721</v>
       </c>
-      <c r="Y10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z10" t="n">
+      <c r="AD10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="n">
         <v>0.2441860465116279</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AF10" t="n">
         <v>0.1918604651162791</v>
       </c>
-      <c r="AB10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC10" t="n">
+      <c r="AG10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1415,78 +1543,90 @@
         <v>0.2409638554216867</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.2409638554216867</v>
       </c>
       <c r="F11" t="n">
+        <v>0.2409638554216867</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.2416107382550335</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.1084337349397591</v>
       </c>
-      <c r="G11" t="n">
+      <c r="J11" t="n">
         <v>0.1686746987951807</v>
       </c>
-      <c r="H11" t="n">
+      <c r="K11" t="n">
         <v>0.1686746987951807</v>
       </c>
-      <c r="I11" t="n">
+      <c r="L11" t="n">
         <v>0.1807228915662651</v>
       </c>
-      <c r="J11" t="n">
-        <v>0.2416107382550335</v>
-      </c>
-      <c r="K11" t="n">
+      <c r="M11" t="n">
+        <v>0.2168674698795181</v>
+      </c>
+      <c r="N11" t="n">
         <v>0.2771084337349398</v>
       </c>
-      <c r="L11" t="n">
+      <c r="O11" t="n">
         <v>0.1084337349397591</v>
       </c>
-      <c r="M11" t="n">
+      <c r="P11" t="n">
         <v>0.2769230769230769</v>
       </c>
-      <c r="N11" t="n">
+      <c r="Q11" t="n">
         <v>0.2769230769230769</v>
       </c>
-      <c r="O11" t="n">
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.2906976744186046</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>1</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.1547619047619048</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.2048192771084337</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.2328767123287672</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.2110091743119266</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.1325301204819277</v>
+      </c>
+      <c r="AF11" t="n">
         <v>0.2168674698795181</v>
       </c>
-      <c r="P11" t="n">
-        <v>0.1084337349397591</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0.2906976744186046</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0.2906976744186046</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" t="n">
-        <v>1</v>
-      </c>
-      <c r="U11" t="n">
-        <v>0.2380952380952381</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0</v>
-      </c>
-      <c r="W11" t="n">
-        <v>0.2328767123287672</v>
-      </c>
-      <c r="X11" t="n">
-        <v>0.2110091743119266</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>0.1325301204819277</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>0.2168674698795181</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC11" t="n">
+      <c r="AG11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1506,78 +1646,90 @@
         <v>0.1861471861471862</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.1861471861471862</v>
       </c>
       <c r="F12" t="n">
+        <v>0.1861471861471862</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.2683982683982684</v>
+      </c>
+      <c r="I12" t="n">
         <v>0.06926406926406925</v>
       </c>
-      <c r="G12" t="n">
+      <c r="J12" t="n">
         <v>0.09956709956709953</v>
       </c>
-      <c r="H12" t="n">
+      <c r="K12" t="n">
         <v>0.09956709956709953</v>
       </c>
-      <c r="I12" t="n">
+      <c r="L12" t="n">
         <v>0.2034632034632035</v>
       </c>
-      <c r="J12" t="n">
-        <v>0.2683982683982684</v>
-      </c>
-      <c r="K12" t="n">
+      <c r="M12" t="n">
+        <v>0.1558441558441559</v>
+      </c>
+      <c r="N12" t="n">
         <v>0.1688311688311688</v>
       </c>
-      <c r="L12" t="n">
+      <c r="O12" t="n">
         <v>0.06926406926406925</v>
       </c>
-      <c r="M12" t="n">
+      <c r="P12" t="n">
         <v>0.2251082251082251</v>
       </c>
-      <c r="N12" t="n">
+      <c r="Q12" t="n">
         <v>0.2251082251082251</v>
       </c>
-      <c r="O12" t="n">
-        <v>0.1558441558441559</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.06926406926406925</v>
-      </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
         <v>0.2727272727272727</v>
       </c>
-      <c r="R12" t="n">
-        <v>0.2727272727272727</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0</v>
-      </c>
       <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
         <v>0.2380952380952381</v>
       </c>
-      <c r="U12" t="n">
-        <v>1</v>
-      </c>
       <c r="V12" t="n">
-        <v>0</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.1601731601731602</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="n">
         <v>0.2510822510822511</v>
       </c>
-      <c r="X12" t="n">
+      <c r="AC12" t="n">
         <v>0.2510822510822511</v>
       </c>
-      <c r="Y12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z12" t="n">
+      <c r="AD12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="n">
         <v>0.1818181818181818</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AF12" t="n">
         <v>0.1471861471861472</v>
       </c>
-      <c r="AB12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC12" t="n">
+      <c r="AG12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1671,6 +1823,18 @@
       <c r="AC13" t="n">
         <v>0</v>
       </c>
+      <c r="AD13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1689,78 +1853,90 @@
         <v>0.1986301369863014</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>0.1986301369863014</v>
       </c>
       <c r="F14" t="n">
+        <v>0.1986301369863014</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.174496644295302</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.08904109589041098</v>
       </c>
-      <c r="G14" t="n">
+      <c r="J14" t="n">
         <v>0.136986301369863</v>
       </c>
-      <c r="H14" t="n">
+      <c r="K14" t="n">
         <v>0.136986301369863</v>
       </c>
-      <c r="I14" t="n">
+      <c r="L14" t="n">
         <v>0.273972602739726</v>
       </c>
-      <c r="J14" t="n">
-        <v>0.174496644295302</v>
-      </c>
-      <c r="K14" t="n">
+      <c r="M14" t="n">
+        <v>0.1917808219178082</v>
+      </c>
+      <c r="N14" t="n">
         <v>0.2397260273972602</v>
       </c>
-      <c r="L14" t="n">
+      <c r="O14" t="n">
         <v>0.08904109589041098</v>
       </c>
-      <c r="M14" t="n">
+      <c r="P14" t="n">
         <v>0.178082191780822</v>
       </c>
-      <c r="N14" t="n">
+      <c r="Q14" t="n">
         <v>0.178082191780822</v>
       </c>
-      <c r="O14" t="n">
-        <v>0.1917808219178082</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0.08904109589041098</v>
-      </c>
-      <c r="Q14" t="n">
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
         <v>0.2674418604651163</v>
       </c>
-      <c r="R14" t="n">
-        <v>0.2674418604651163</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0</v>
-      </c>
       <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
         <v>0.2328767123287672</v>
       </c>
-      <c r="U14" t="n">
+      <c r="V14" t="n">
+        <v>0.2328767123287672</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="n">
         <v>0.2510822510822511</v>
       </c>
-      <c r="V14" t="n">
-        <v>0</v>
-      </c>
-      <c r="W14" t="n">
-        <v>1</v>
-      </c>
-      <c r="X14" t="n">
+      <c r="Z14" t="n">
+        <v>0.2123287671232876</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC14" t="n">
         <v>0.2671232876712328</v>
       </c>
-      <c r="Y14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z14" t="n">
+      <c r="AD14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE14" t="n">
         <v>0.2534246575342466</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AF14" t="n">
         <v>0.1986301369863014</v>
       </c>
-      <c r="AB14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC14" t="n">
+      <c r="AG14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1781,78 +1957,90 @@
         <v>0.2477064220183486</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.2477064220183486</v>
       </c>
       <c r="F15" t="n">
+        <v>0.2477064220183486</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.2885906040268457</v>
+      </c>
+      <c r="I15" t="n">
         <v>0.1100917431192661</v>
       </c>
-      <c r="G15" t="n">
+      <c r="J15" t="n">
         <v>0.1743119266055045</v>
       </c>
-      <c r="H15" t="n">
+      <c r="K15" t="n">
         <v>0.1743119266055045</v>
       </c>
-      <c r="I15" t="n">
+      <c r="L15" t="n">
         <v>0.3027522935779816</v>
       </c>
-      <c r="J15" t="n">
-        <v>0.2885906040268457</v>
-      </c>
-      <c r="K15" t="n">
+      <c r="M15" t="n">
+        <v>0.2568807339449541</v>
+      </c>
+      <c r="N15" t="n">
         <v>0.2752293577981652</v>
       </c>
-      <c r="L15" t="n">
+      <c r="O15" t="n">
         <v>0.1100917431192661</v>
       </c>
-      <c r="M15" t="n">
+      <c r="P15" t="n">
         <v>0.2461538461538462</v>
       </c>
-      <c r="N15" t="n">
+      <c r="Q15" t="n">
         <v>0.2461538461538462</v>
       </c>
-      <c r="O15" t="n">
-        <v>0.2568807339449541</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0.1100917431192661</v>
-      </c>
-      <c r="Q15" t="n">
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
         <v>0.2558139534883721</v>
       </c>
-      <c r="R15" t="n">
-        <v>0.2558139534883721</v>
-      </c>
-      <c r="S15" t="n">
-        <v>0</v>
-      </c>
       <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
         <v>0.2110091743119266</v>
       </c>
-      <c r="U15" t="n">
+      <c r="V15" t="n">
+        <v>0.2385321100917431</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="n">
         <v>0.2510822510822511</v>
       </c>
-      <c r="V15" t="n">
-        <v>0</v>
-      </c>
-      <c r="W15" t="n">
+      <c r="Z15" t="n">
+        <v>0.2935779816513762</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="n">
         <v>0.2671232876712328</v>
       </c>
-      <c r="X15" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z15" t="n">
+      <c r="AC15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="n">
         <v>0.2385321100917431</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AF15" t="n">
         <v>0.2752293577981652</v>
       </c>
-      <c r="AB15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC15" t="n">
+      <c r="AG15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1914,37 +2102,49 @@
         <v>0</v>
       </c>
       <c r="S16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
       </c>
       <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="W16" t="n">
-        <v>0</v>
-      </c>
       <c r="X16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z16" t="n">
         <v>0</v>
       </c>
       <c r="AA16" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="AB16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG16" t="n">
         <v>0.6470588235294117</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1963,78 +2163,90 @@
         <v>0.1975308641975309</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.1975308641975309</v>
       </c>
       <c r="F17" t="n">
+        <v>0.1975308641975309</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.2348993288590604</v>
+      </c>
+      <c r="I17" t="n">
         <v>0.1358024691358025</v>
       </c>
-      <c r="G17" t="n">
+      <c r="J17" t="n">
         <v>0.3580246913580247</v>
       </c>
-      <c r="H17" t="n">
+      <c r="K17" t="n">
         <v>0.3580246913580247</v>
       </c>
-      <c r="I17" t="n">
+      <c r="L17" t="n">
         <v>0.2592592592592593</v>
       </c>
-      <c r="J17" t="n">
-        <v>0.2348993288590604</v>
-      </c>
-      <c r="K17" t="n">
+      <c r="M17" t="n">
         <v>0.1975308641975309</v>
       </c>
-      <c r="L17" t="n">
+      <c r="N17" t="n">
+        <v>0.1975308641975309</v>
+      </c>
+      <c r="O17" t="n">
         <v>0.1358024691358025</v>
       </c>
-      <c r="M17" t="n">
+      <c r="P17" t="n">
         <v>0.2076923076923077</v>
       </c>
-      <c r="N17" t="n">
+      <c r="Q17" t="n">
         <v>0.2076923076923077</v>
       </c>
-      <c r="O17" t="n">
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.2441860465116279</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.1325301204819277</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.1428571428571429</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="Z17" t="n">
         <v>0.1975308641975309</v>
       </c>
-      <c r="P17" t="n">
-        <v>0.1358024691358025</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0.2441860465116279</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0.2441860465116279</v>
-      </c>
-      <c r="S17" t="n">
-        <v>0</v>
-      </c>
-      <c r="T17" t="n">
-        <v>0.1325301204819277</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.1818181818181818</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0</v>
-      </c>
-      <c r="W17" t="n">
+      <c r="AA17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" t="n">
         <v>0.2534246575342466</v>
       </c>
-      <c r="X17" t="n">
+      <c r="AC17" t="n">
         <v>0.2385321100917431</v>
       </c>
-      <c r="Y17" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA17" t="n">
+      <c r="AD17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF17" t="n">
         <v>0.3950617283950617</v>
       </c>
-      <c r="AB17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC17" t="n">
+      <c r="AG17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2054,78 +2266,90 @@
         <v>0.2380952380952381</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="F18" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.2013422818791947</v>
+      </c>
+      <c r="I18" t="n">
         <v>0.2115384615384616</v>
       </c>
-      <c r="G18" t="n">
+      <c r="J18" t="n">
         <v>0.25</v>
       </c>
-      <c r="H18" t="n">
+      <c r="K18" t="n">
         <v>0.25</v>
       </c>
-      <c r="I18" t="n">
+      <c r="L18" t="n">
         <v>0.2222222222222222</v>
       </c>
-      <c r="J18" t="n">
-        <v>0.2013422818791947</v>
-      </c>
-      <c r="K18" t="n">
+      <c r="M18" t="n">
+        <v>0.1403508771929824</v>
+      </c>
+      <c r="N18" t="n">
         <v>0.2459016393442623</v>
       </c>
-      <c r="L18" t="n">
+      <c r="O18" t="n">
         <v>0.2115384615384616</v>
       </c>
-      <c r="M18" t="n">
+      <c r="P18" t="n">
         <v>0.1923076923076923</v>
       </c>
-      <c r="N18" t="n">
+      <c r="Q18" t="n">
         <v>0.1923076923076923</v>
       </c>
-      <c r="O18" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0.2115384615384616</v>
-      </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
         <v>0.1918604651162791</v>
       </c>
-      <c r="R18" t="n">
-        <v>0.1918604651162791</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0</v>
-      </c>
       <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
         <v>0.2168674698795181</v>
       </c>
-      <c r="U18" t="n">
+      <c r="V18" t="n">
+        <v>0.2023809523809523</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="n">
         <v>0.1471861471861472</v>
       </c>
-      <c r="V18" t="n">
-        <v>0</v>
-      </c>
-      <c r="W18" t="n">
+      <c r="Z18" t="n">
+        <v>0.1774193548387096</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" t="n">
         <v>0.1986301369863014</v>
       </c>
-      <c r="X18" t="n">
+      <c r="AC18" t="n">
         <v>0.2752293577981652</v>
       </c>
-      <c r="Y18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="n">
+      <c r="AD18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE18" t="n">
         <v>0.3950617283950617</v>
       </c>
-      <c r="AA18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC18" t="n">
+      <c r="AF18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2187,37 +2411,49 @@
         <v>0</v>
       </c>
       <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="T19" t="n">
-        <v>0</v>
-      </c>
       <c r="U19" t="n">
         <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="Y19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD19" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="Z19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>0</v>
+      <c r="AE19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -2310,6 +2546,18 @@
       <c r="AC20" t="n">
         <v>0</v>
       </c>
+      <c r="AD20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -2327,13 +2575,13 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2366,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="R21" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -2399,7 +2647,19 @@
         <v>0</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.625</v>
+        <v>0</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2492,6 +2752,18 @@
       <c r="AC22" t="n">
         <v>0</v>
       </c>
+      <c r="AD22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -2551,37 +2823,49 @@
         <v>0</v>
       </c>
       <c r="S23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" t="n">
         <v>0</v>
       </c>
       <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="W23" t="n">
-        <v>0</v>
-      </c>
       <c r="X23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z23" t="n">
         <v>0</v>
       </c>
       <c r="AA23" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="AB23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG23" t="n">
         <v>0.6470588235294117</v>
-      </c>
-      <c r="AC23" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2642,37 +2926,49 @@
         <v>0</v>
       </c>
       <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="T24" t="n">
-        <v>0</v>
-      </c>
       <c r="U24" t="n">
         <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="Y24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD24" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="Z24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC24" t="n">
-        <v>0</v>
+      <c r="AE24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -2691,14 +2987,14 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
         <v>0.625</v>
       </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0</v>
-      </c>
       <c r="H25" t="n">
         <v>0</v>
       </c>
@@ -2730,7 +3026,7 @@
         <v>0</v>
       </c>
       <c r="R25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25" t="n">
         <v>0</v>
@@ -2763,7 +3059,19 @@
         <v>0</v>
       </c>
       <c r="AC25" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Docker file and dependencies
</commit_message>
<xml_diff>
--- a/similarity_matrix.xlsx
+++ b/similarity_matrix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG25"/>
+  <dimension ref="A1:AD25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,32 +446,32 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>activity1-1 (Rapid initial evaluation for airway, breathing, and circulation)</t>
+          <t>activity1 (Rapid initial evaluation for airway, breathing, and circulation)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>activity1-2 (Rapid initial evaluation for airway, breathing, and circulation)</t>
+          <t>parallelgateway1 (Parallel Gateway)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>activity1-3 (Rapid initial evaluation for airway, breathing, and circulation)</t>
+          <t>dummy_Flow_2 ((dummy branch entry))</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>parallelgateway1 (Parallel Gateway)</t>
+          <t>activity2-1 (neurological examination to determine focal neurological deficits and assess stroke severity on a standardized stroke scale (NIHSS or CNS for stroke))</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>activity2 (neurological examination to determine focal neurological deficits and assess stroke severity on a standardized stroke scale (NIHSS or CNS for stroke))</t>
+          <t>activity2-2 (neurological examination to determine focal neurological deficits and assess stroke severity on a standardized stroke scale (NIHSS or CNS for stroke))</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>dummy_Flow_4 ((dummy branch entry))</t>
+          <t>dummy_Flow_5 ((dummy branch entry))</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -491,12 +491,12 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>activity4-1 (Chest x-ray without delay for for thrombolysis assessment)</t>
+          <t>activity5 (ECG to detect atrial fibrillation and other acute arrhythmias)</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>activity5 (ECG to detect atrial fibrillation and other acute arrhythmias)</t>
+          <t>activity6 (Chest x-ray without delay for for thrombolysis assessment)</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -506,96 +506,77 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>activity6-1 (Blood work:
- CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
+          <t>activity7-1 (Blood work: CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>activity6-2 (Blood work:
- CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
+          <t>activity7-2 (Blood work: CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>dummy_Flow_12 ((dummy branch entry))</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>activity8 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>exclusivegateway1 (Exclusive Gateway)</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>activity9 (Monitor patient closely and swallowing ability screened when clinically appropriate)</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>activity10 (Full clinical assessment of the patient's swallowing ability by an expert (by a speech-language pathologist or appropriately trained specialist who would advise on swallowing ability and the required consistency of diet and fluids))</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>exclusivegateway1Join (Exclusive Merge)</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>activity11 (Give patients appropriate cross-continuum secondary prevention assessments and therapies (All patients, whether admitted or discharged from the ED))</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>activity12 (Use a standard triage tool to determine the appropriate location for the care of patients (Patients with TIA))</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>exclusivegateway2 (Exclusive Gateway)</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>activity13 (Immediate vascular imaging of the neck arteries (carotid ultrasound, CTA, or MRA))</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>activity14 (Vascular imaging of the brain and neck arteries ASAP)</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>exclusivegateway2Join (Exclusive Merge)</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
           <t>parallelgateway1Join (Parallel Merge)</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>activity8 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>exclusivegateway1 (Exclusive Gateway)</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>activity9 (Monitor patient closely and swallowing ability screened when clinically appropriate)</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>activity10 (Proceed with further assessment as indicated (Role: medical staff; Objects: patient))</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>exclusivegateway1Join (Exclusive Merge)</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>exclusivegateway2 (Exclusive Gateway)</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>activity11 (Full clinical assessment of the patient's swallowing ability by an expert (by a speech-language pathologist or appropriately trained specialist who would advise on swallowing ability and the required consistency of diet and fluids))</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>activity12 (Continue standard care (Role: medical staff; Objects: patient))</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>exclusivegateway2Join (Exclusive Merge)</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>activity13 (Give patients appropriate cross-continuum secondary prevention assessments and therapies
-(All patients, whether admitted or discharged from the ED)</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>activity14 (Use a standard triage tool to determine the appropriate location for the care of patients
-(Patients with TIA))</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>exclusivegateway3 (Exclusive Gateway)</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>activity15 (Immediate vascular imaging of the neck arteries (carotid ultrasound, CTA, or MRA))</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>activity16 (Vascular imaging of the brain and neck arteries ASAP)</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>exclusivegateway3Join (Exclusive Merge)</t>
         </is>
       </c>
     </row>
@@ -692,15 +673,6 @@
       <c r="AD2" t="n">
         <v>0</v>
       </c>
-      <c r="AE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -718,13 +690,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0.1746031746031746</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.214765100671141</v>
       </c>
       <c r="H3" t="n">
         <v>0.214765100671141</v>
@@ -751,13 +723,13 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="P3" t="n">
-        <v>0.2307692307692307</v>
+        <v>0.2325581395348837</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.2307692307692307</v>
+        <v>0.2325581395348837</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>0.1746031746031746</v>
       </c>
       <c r="S3" t="n">
         <v>0.2209302325581395</v>
@@ -769,39 +741,30 @@
         <v>0.2409638554216867</v>
       </c>
       <c r="V3" t="n">
-        <v>0.2261904761904762</v>
+        <v>0.1861471861471862</v>
       </c>
       <c r="W3" t="n">
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>0.1972789115646258</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.1861471861471862</v>
+        <v>0.2568807339449541</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.1587301587301587</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>0</v>
+        <v>0.1975308641975309</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.1986301369863014</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.2477064220183486</v>
+        <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0.1975308641975309</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>0.2380952380952381</v>
-      </c>
-      <c r="AG3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -821,13 +784,13 @@
         <v>0.214765100671141</v>
       </c>
       <c r="E4" t="n">
-        <v>0.214765100671141</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.214765100671141</v>
+        <v>0.09395973154362414</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -845,22 +808,22 @@
         <v>0.2080536912751678</v>
       </c>
       <c r="M4" t="n">
+        <v>0.2348993288590604</v>
+      </c>
+      <c r="N4" t="n">
         <v>0.1879194630872483</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.2348993288590604</v>
       </c>
       <c r="O4" t="n">
         <v>0.09395973154362414</v>
       </c>
       <c r="P4" t="n">
-        <v>0.174496644295302</v>
+        <v>0.1812080536912751</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.174496644295302</v>
+        <v>0.1812080536912751</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>0.09395973154362414</v>
       </c>
       <c r="S4" t="n">
         <v>0.2325581395348837</v>
@@ -872,39 +835,30 @@
         <v>0.2416107382550335</v>
       </c>
       <c r="V4" t="n">
-        <v>0.2281879194630873</v>
+        <v>0.2683982683982684</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>0.1812080536912751</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.2683982683982684</v>
+        <v>0.2953020134228188</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.1946308724832215</v>
+        <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>0.2348993288590604</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.174496644295302</v>
+        <v>0.2013422818791947</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.2885906040268457</v>
+        <v>0</v>
       </c>
       <c r="AD4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0.2348993288590604</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0.2013422818791947</v>
-      </c>
-      <c r="AG4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -924,13 +878,13 @@
         <v>0.253968253968254</v>
       </c>
       <c r="E5" t="n">
-        <v>0.253968253968254</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.253968253968254</v>
+        <v>0.2571428571428571</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.1476510067114094</v>
       </c>
       <c r="H5" t="n">
         <v>0.1476510067114094</v>
@@ -948,22 +902,22 @@
         <v>0.3055555555555556</v>
       </c>
       <c r="M5" t="n">
+        <v>0.2295081967213115</v>
+      </c>
+      <c r="N5" t="n">
         <v>0.1403508771929824</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.2295081967213115</v>
       </c>
       <c r="O5" t="n">
         <v>0.2571428571428571</v>
       </c>
       <c r="P5" t="n">
-        <v>0.1538461538461539</v>
+        <v>0.1550387596899225</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1538461538461539</v>
+        <v>0.1550387596899225</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>0.2571428571428571</v>
       </c>
       <c r="S5" t="n">
         <v>0.1279069767441861</v>
@@ -975,39 +929,30 @@
         <v>0.1686746987951807</v>
       </c>
       <c r="V5" t="n">
-        <v>0.1904761904761905</v>
+        <v>0.09956709956709953</v>
       </c>
       <c r="W5" t="n">
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>0.1428571428571429</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.09956709956709953</v>
+        <v>0.1743119266055045</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.1774193548387096</v>
+        <v>0</v>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>0.3580246913580247</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.136986301369863</v>
+        <v>0.25</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1743119266055045</v>
+        <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>0.3580246913580247</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="AG5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1027,13 +972,13 @@
         <v>0.2361111111111112</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2361111111111112</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2361111111111112</v>
+        <v>0.1388888888888888</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.2080536912751678</v>
       </c>
       <c r="H6" t="n">
         <v>0.2080536912751678</v>
@@ -1051,22 +996,22 @@
         <v>1</v>
       </c>
       <c r="M6" t="n">
+        <v>0.2638888888888888</v>
+      </c>
+      <c r="N6" t="n">
         <v>0.2222222222222222</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.2638888888888888</v>
       </c>
       <c r="O6" t="n">
         <v>0.1388888888888888</v>
       </c>
       <c r="P6" t="n">
-        <v>0.2307692307692307</v>
+        <v>0.2325581395348837</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.2307692307692307</v>
+        <v>0.2325581395348837</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>0.1388888888888888</v>
       </c>
       <c r="S6" t="n">
         <v>0.2209302325581395</v>
@@ -1078,39 +1023,30 @@
         <v>0.1807228915662651</v>
       </c>
       <c r="V6" t="n">
-        <v>0.2142857142857143</v>
+        <v>0.2034632034632035</v>
       </c>
       <c r="W6" t="n">
         <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>0</v>
+        <v>0.2721088435374149</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.2034632034632035</v>
+        <v>0.3119266055045872</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AA6" t="n">
-        <v>0</v>
+        <v>0.2592592592592593</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.273972602739726</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.3027522935779816</v>
+        <v>0</v>
       </c>
       <c r="AD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0.2592592592592593</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="AG6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1130,13 +1066,13 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1746031746031746</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1746031746031746</v>
+        <v>0.180327868852459</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.2348993288590604</v>
       </c>
       <c r="H7" t="n">
         <v>0.2348993288590604</v>
@@ -1154,22 +1090,22 @@
         <v>0.2638888888888888</v>
       </c>
       <c r="M7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" t="n">
         <v>0.180327868852459</v>
-      </c>
-      <c r="N7" t="n">
-        <v>1</v>
       </c>
       <c r="O7" t="n">
         <v>0.180327868852459</v>
       </c>
       <c r="P7" t="n">
-        <v>0.2384615384615385</v>
+        <v>0.248062015503876</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2384615384615385</v>
+        <v>0.248062015503876</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>0.180327868852459</v>
       </c>
       <c r="S7" t="n">
         <v>0.1976744186046512</v>
@@ -1181,39 +1117,30 @@
         <v>0.2771084337349398</v>
       </c>
       <c r="V7" t="n">
-        <v>0.2023809523809523</v>
+        <v>0.1688311688311688</v>
       </c>
       <c r="W7" t="n">
         <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>0</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.1688311688311688</v>
+        <v>0.2844036697247706</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.1451612903225806</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
-        <v>0</v>
+        <v>0.1975308641975309</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.2397260273972602</v>
+        <v>0.2459016393442623</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.2752293577981652</v>
+        <v>0</v>
       </c>
       <c r="AD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0.1975308641975309</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>0.2459016393442623</v>
-      </c>
-      <c r="AG7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1233,13 +1160,13 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1746031746031746</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1746031746031746</v>
+        <v>0.1403508771929824</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.1879194630872483</v>
       </c>
       <c r="H8" t="n">
         <v>0.1879194630872483</v>
@@ -1257,22 +1184,22 @@
         <v>0.2222222222222222</v>
       </c>
       <c r="M8" t="n">
+        <v>0.180327868852459</v>
+      </c>
+      <c r="N8" t="n">
         <v>1</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.180327868852459</v>
       </c>
       <c r="O8" t="n">
         <v>0.1403508771929824</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2230769230769231</v>
+        <v>0.2248062015503876</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2230769230769231</v>
+        <v>0.2248062015503876</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>0.1403508771929824</v>
       </c>
       <c r="S8" t="n">
         <v>0.2034883720930233</v>
@@ -1284,39 +1211,30 @@
         <v>0.2168674698795181</v>
       </c>
       <c r="V8" t="n">
-        <v>0.2023809523809523</v>
+        <v>0.1558441558441559</v>
       </c>
       <c r="W8" t="n">
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>0</v>
+        <v>0.1972789115646258</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.1558441558441559</v>
+        <v>0.2660550458715596</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.1612903225806451</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>0</v>
+        <v>0.1975308641975309</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.1917808219178082</v>
+        <v>0.1403508771929824</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.2568807339449541</v>
+        <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>0.1975308641975309</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="AG8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1337,13 +1255,13 @@
         <v>0.2307692307692307</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2307692307692307</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2307692307692307</v>
+        <v>0.1153846153846154</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.174496644295302</v>
       </c>
       <c r="H9" t="n">
         <v>0.174496644295302</v>
@@ -1361,22 +1279,22 @@
         <v>0.2307692307692307</v>
       </c>
       <c r="M9" t="n">
+        <v>0.2384615384615385</v>
+      </c>
+      <c r="N9" t="n">
         <v>0.2230769230769231</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.2384615384615385</v>
       </c>
       <c r="O9" t="n">
         <v>0.1153846153846154</v>
       </c>
       <c r="P9" t="n">
-        <v>1</v>
+        <v>0.9846153846153847</v>
       </c>
       <c r="Q9" t="n">
-        <v>1</v>
+        <v>0.9846153846153847</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>0.1153846153846154</v>
       </c>
       <c r="S9" t="n">
         <v>0.2441860465116279</v>
@@ -1388,39 +1306,30 @@
         <v>0.2769230769230769</v>
       </c>
       <c r="V9" t="n">
-        <v>0.2230769230769231</v>
+        <v>0.2251082251082251</v>
       </c>
       <c r="W9" t="n">
         <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>0</v>
+        <v>0.1904761904761905</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.2251082251082251</v>
+        <v>0.2538461538461538</v>
       </c>
       <c r="Z9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="n">
         <v>0.2076923076923077</v>
       </c>
-      <c r="AA9" t="n">
-        <v>0</v>
-      </c>
       <c r="AB9" t="n">
-        <v>0.178082191780822</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.2461538461538462</v>
+        <v>0</v>
       </c>
       <c r="AD9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>0.2076923076923077</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>0.1923076923076923</v>
-      </c>
-      <c r="AG9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1440,13 +1349,13 @@
         <v>0.2209302325581395</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2209302325581395</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2209302325581395</v>
+        <v>0.07558139534883723</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.2325581395348837</v>
       </c>
       <c r="H10" t="n">
         <v>0.2325581395348837</v>
@@ -1464,22 +1373,22 @@
         <v>0.2209302325581395</v>
       </c>
       <c r="M10" t="n">
+        <v>0.1976744186046512</v>
+      </c>
+      <c r="N10" t="n">
         <v>0.2034883720930233</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.1976744186046512</v>
       </c>
       <c r="O10" t="n">
         <v>0.07558139534883723</v>
       </c>
       <c r="P10" t="n">
-        <v>0.2441860465116279</v>
+        <v>0.25</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.2441860465116279</v>
+        <v>0.25</v>
       </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>0.07558139534883723</v>
       </c>
       <c r="S10" t="n">
         <v>1</v>
@@ -1491,39 +1400,30 @@
         <v>0.2906976744186046</v>
       </c>
       <c r="V10" t="n">
-        <v>0.2209302325581395</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="W10" t="n">
         <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>0</v>
+        <v>0.2674418604651163</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.2616279069767442</v>
       </c>
       <c r="Z10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0.2441860465116279</v>
+      </c>
+      <c r="AB10" t="n">
         <v>0.1918604651162791</v>
       </c>
-      <c r="AA10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>0.2674418604651163</v>
-      </c>
       <c r="AC10" t="n">
-        <v>0.2558139534883721</v>
+        <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE10" t="n">
-        <v>0.2441860465116279</v>
-      </c>
-      <c r="AF10" t="n">
-        <v>0.1918604651162791</v>
-      </c>
-      <c r="AG10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1543,13 +1443,13 @@
         <v>0.2409638554216867</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2409638554216867</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2409638554216867</v>
+        <v>0.1084337349397591</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.2416107382550335</v>
       </c>
       <c r="H11" t="n">
         <v>0.2416107382550335</v>
@@ -1567,22 +1467,22 @@
         <v>0.1807228915662651</v>
       </c>
       <c r="M11" t="n">
+        <v>0.2771084337349398</v>
+      </c>
+      <c r="N11" t="n">
         <v>0.2168674698795181</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.2771084337349398</v>
       </c>
       <c r="O11" t="n">
         <v>0.1084337349397591</v>
       </c>
       <c r="P11" t="n">
-        <v>0.2769230769230769</v>
+        <v>0.2790697674418605</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.2769230769230769</v>
+        <v>0.2790697674418605</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>0.1084337349397591</v>
       </c>
       <c r="S11" t="n">
         <v>0.2906976744186046</v>
@@ -1594,39 +1494,30 @@
         <v>1</v>
       </c>
       <c r="V11" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="W11" t="n">
         <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>0</v>
+        <v>0.2312925170068028</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.2380952380952381</v>
+        <v>0.2110091743119266</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.2048192771084337</v>
+        <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>0</v>
+        <v>0.1325301204819277</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.2328767123287672</v>
+        <v>0.2168674698795181</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.2110091743119266</v>
+        <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>0.1325301204819277</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>0.2168674698795181</v>
-      </c>
-      <c r="AG11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1646,13 +1537,13 @@
         <v>0.1861471861471862</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1861471861471862</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1861471861471862</v>
+        <v>0.06926406926406925</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.2683982683982684</v>
       </c>
       <c r="H12" t="n">
         <v>0.2683982683982684</v>
@@ -1670,22 +1561,22 @@
         <v>0.2034632034632035</v>
       </c>
       <c r="M12" t="n">
+        <v>0.1688311688311688</v>
+      </c>
+      <c r="N12" t="n">
         <v>0.1558441558441559</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.1688311688311688</v>
       </c>
       <c r="O12" t="n">
         <v>0.06926406926406925</v>
       </c>
       <c r="P12" t="n">
-        <v>0.2251082251082251</v>
+        <v>0.2294372294372294</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.2251082251082251</v>
+        <v>0.2294372294372294</v>
       </c>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>0.06926406926406925</v>
       </c>
       <c r="S12" t="n">
         <v>0.2727272727272727</v>
@@ -1697,39 +1588,30 @@
         <v>0.2380952380952381</v>
       </c>
       <c r="V12" t="n">
+        <v>1</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.2597402597402597</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.2554112554112554</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="n">
         <v>0.1818181818181818</v>
       </c>
-      <c r="W12" t="n">
-        <v>0</v>
-      </c>
-      <c r="X12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>0.1601731601731602</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>0</v>
-      </c>
       <c r="AB12" t="n">
-        <v>0.2510822510822511</v>
+        <v>0.1471861471861472</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.2510822510822511</v>
+        <v>0</v>
       </c>
       <c r="AD12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>0.1818181818181818</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>0.1471861471861472</v>
-      </c>
-      <c r="AG12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1826,15 +1708,6 @@
       <c r="AD13" t="n">
         <v>0</v>
       </c>
-      <c r="AE13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG13" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1853,13 +1726,13 @@
         <v>0.1986301369863014</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1986301369863014</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1986301369863014</v>
+        <v>0.08904109589041098</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.174496644295302</v>
       </c>
       <c r="H14" t="n">
         <v>0.174496644295302</v>
@@ -1877,22 +1750,22 @@
         <v>0.273972602739726</v>
       </c>
       <c r="M14" t="n">
+        <v>0.2397260273972602</v>
+      </c>
+      <c r="N14" t="n">
         <v>0.1917808219178082</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.2397260273972602</v>
       </c>
       <c r="O14" t="n">
         <v>0.08904109589041098</v>
       </c>
       <c r="P14" t="n">
-        <v>0.178082191780822</v>
+        <v>0.184931506849315</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.178082191780822</v>
+        <v>0.184931506849315</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>0.08904109589041098</v>
       </c>
       <c r="S14" t="n">
         <v>0.2674418604651163</v>
@@ -1904,39 +1777,30 @@
         <v>0.2328767123287672</v>
       </c>
       <c r="V14" t="n">
-        <v>0.2328767123287672</v>
+        <v>0.2510822510822511</v>
       </c>
       <c r="W14" t="n">
         <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>0</v>
+        <v>0.9863945578231292</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.2510822510822511</v>
+        <v>0.273972602739726</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.2123287671232876</v>
+        <v>0</v>
       </c>
       <c r="AA14" t="n">
-        <v>0</v>
+        <v>0.2534246575342466</v>
       </c>
       <c r="AB14" t="n">
-        <v>1</v>
+        <v>0.1986301369863014</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.2671232876712328</v>
+        <v>0</v>
       </c>
       <c r="AD14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE14" t="n">
-        <v>0.2534246575342466</v>
-      </c>
-      <c r="AF14" t="n">
-        <v>0.1986301369863014</v>
-      </c>
-      <c r="AG14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1957,13 +1821,13 @@
         <v>0.2477064220183486</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2477064220183486</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2477064220183486</v>
+        <v>0.1100917431192661</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.2885906040268457</v>
       </c>
       <c r="H15" t="n">
         <v>0.2885906040268457</v>
@@ -1981,22 +1845,22 @@
         <v>0.3027522935779816</v>
       </c>
       <c r="M15" t="n">
+        <v>0.2752293577981652</v>
+      </c>
+      <c r="N15" t="n">
         <v>0.2568807339449541</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0.2752293577981652</v>
       </c>
       <c r="O15" t="n">
         <v>0.1100917431192661</v>
       </c>
       <c r="P15" t="n">
-        <v>0.2461538461538462</v>
+        <v>0.2403100775193798</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.2461538461538462</v>
+        <v>0.2403100775193798</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>0.1100917431192661</v>
       </c>
       <c r="S15" t="n">
         <v>0.2558139534883721</v>
@@ -2008,39 +1872,30 @@
         <v>0.2110091743119266</v>
       </c>
       <c r="V15" t="n">
+        <v>0.2510822510822511</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0.2789115646258503</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.9908256880733946</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="n">
         <v>0.2385321100917431</v>
       </c>
-      <c r="W15" t="n">
-        <v>0</v>
-      </c>
-      <c r="X15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>0.2510822510822511</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>0.2935779816513762</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>0</v>
-      </c>
       <c r="AB15" t="n">
-        <v>0.2671232876712328</v>
+        <v>0.2752293577981652</v>
       </c>
       <c r="AC15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>0.2385321100917431</v>
-      </c>
-      <c r="AF15" t="n">
-        <v>0.2752293577981652</v>
-      </c>
-      <c r="AG15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2117,34 +1972,25 @@
         <v>0.6470588235294117</v>
       </c>
       <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="n">
         <v>1</v>
       </c>
-      <c r="Y16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>0</v>
-      </c>
       <c r="AA16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="AB16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>0</v>
-      </c>
       <c r="AD16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG16" t="n">
-        <v>0.6470588235294117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2163,13 +2009,13 @@
         <v>0.1975308641975309</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1975308641975309</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1975308641975309</v>
+        <v>0.1358024691358025</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>0.2348993288590604</v>
       </c>
       <c r="H17" t="n">
         <v>0.2348993288590604</v>
@@ -2196,13 +2042,13 @@
         <v>0.1358024691358025</v>
       </c>
       <c r="P17" t="n">
-        <v>0.2076923076923077</v>
+        <v>0.2093023255813954</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.2076923076923077</v>
+        <v>0.2093023255813954</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>0.1358024691358025</v>
       </c>
       <c r="S17" t="n">
         <v>0.2441860465116279</v>
@@ -2214,39 +2060,30 @@
         <v>0.1325301204819277</v>
       </c>
       <c r="V17" t="n">
-        <v>0.1428571428571429</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="W17" t="n">
         <v>0</v>
       </c>
       <c r="X17" t="n">
-        <v>0</v>
+        <v>0.2653061224489796</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.1818181818181818</v>
+        <v>0.2477064220183486</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.1975308641975309</v>
+        <v>0</v>
       </c>
       <c r="AA17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.2534246575342466</v>
+        <v>0.3950617283950617</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.2385321100917431</v>
+        <v>0</v>
       </c>
       <c r="AD17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF17" t="n">
-        <v>0.3950617283950617</v>
-      </c>
-      <c r="AG17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2266,13 +2103,13 @@
         <v>0.2380952380952381</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2380952380952381</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2380952380952381</v>
+        <v>0.2115384615384616</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.2013422818791947</v>
       </c>
       <c r="H18" t="n">
         <v>0.2013422818791947</v>
@@ -2290,22 +2127,22 @@
         <v>0.2222222222222222</v>
       </c>
       <c r="M18" t="n">
+        <v>0.2459016393442623</v>
+      </c>
+      <c r="N18" t="n">
         <v>0.1403508771929824</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0.2459016393442623</v>
       </c>
       <c r="O18" t="n">
         <v>0.2115384615384616</v>
       </c>
       <c r="P18" t="n">
-        <v>0.1923076923076923</v>
+        <v>0.1937984496124031</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.1923076923076923</v>
+        <v>0.1937984496124031</v>
       </c>
       <c r="R18" t="n">
-        <v>0</v>
+        <v>0.2115384615384616</v>
       </c>
       <c r="S18" t="n">
         <v>0.1918604651162791</v>
@@ -2317,39 +2154,30 @@
         <v>0.2168674698795181</v>
       </c>
       <c r="V18" t="n">
-        <v>0.2023809523809523</v>
+        <v>0.1471861471861472</v>
       </c>
       <c r="W18" t="n">
         <v>0</v>
       </c>
       <c r="X18" t="n">
-        <v>0</v>
+        <v>0.1972789115646258</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.1471861471861472</v>
+        <v>0.2752293577981652</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.1774193548387096</v>
+        <v>0</v>
       </c>
       <c r="AA18" t="n">
-        <v>0</v>
+        <v>0.3950617283950617</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.1986301369863014</v>
+        <v>1</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.2752293577981652</v>
+        <v>0</v>
       </c>
       <c r="AD18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE18" t="n">
-        <v>0.3950617283950617</v>
-      </c>
-      <c r="AF18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2426,34 +2254,25 @@
         <v>1</v>
       </c>
       <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="Y19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>0</v>
-      </c>
       <c r="AA19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="n">
         <v>1</v>
       </c>
-      <c r="AB19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>0</v>
-      </c>
       <c r="AD19" t="n">
-        <v>0.6470588235294117</v>
-      </c>
-      <c r="AE19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2549,15 +2368,6 @@
       <c r="AD20" t="n">
         <v>0</v>
       </c>
-      <c r="AE20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -2575,13 +2385,13 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -2614,52 +2424,43 @@
         <v>0</v>
       </c>
       <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD21" t="n">
         <v>0.625</v>
-      </c>
-      <c r="S21" t="n">
-        <v>0</v>
-      </c>
-      <c r="T21" t="n">
-        <v>0</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0</v>
-      </c>
-      <c r="V21" t="n">
-        <v>0</v>
-      </c>
-      <c r="W21" t="n">
-        <v>0</v>
-      </c>
-      <c r="X21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG21" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2755,15 +2556,6 @@
       <c r="AD22" t="n">
         <v>0</v>
       </c>
-      <c r="AE22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG22" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -2838,34 +2630,25 @@
         <v>0.6470588235294117</v>
       </c>
       <c r="X23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="n">
         <v>1</v>
       </c>
-      <c r="Y23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z23" t="n">
-        <v>0</v>
-      </c>
       <c r="AA23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="AB23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC23" t="n">
-        <v>0</v>
-      </c>
       <c r="AD23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG23" t="n">
-        <v>0.6470588235294117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2941,34 +2724,25 @@
         <v>1</v>
       </c>
       <c r="X24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="Y24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>0</v>
-      </c>
       <c r="AA24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="n">
         <v>1</v>
       </c>
-      <c r="AB24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC24" t="n">
-        <v>0</v>
-      </c>
       <c r="AD24" t="n">
-        <v>0.6470588235294117</v>
-      </c>
-      <c r="AE24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2987,13 +2761,13 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -3026,52 +2800,43 @@
         <v>0</v>
       </c>
       <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD25" t="n">
         <v>1</v>
-      </c>
-      <c r="S25" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" t="n">
-        <v>0</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" t="n">
-        <v>0</v>
-      </c>
-      <c r="W25" t="n">
-        <v>0</v>
-      </c>
-      <c r="X25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG25" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved UI for results' readability
</commit_message>
<xml_diff>
--- a/similarity_matrix.xlsx
+++ b/similarity_matrix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD25"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,147 +436,145 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>StartEvent_1 (Start)</t>
+          <t>id64c58fce-5b77-4277-bd6e-325a3b70a3b6 (Immediate vascular imaging of the neck arteries (carotid ultrasound, CTA, or MRA))</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EndEvent_1 (End)</t>
+          <t>id902a9355-167c-448e-af72-0fee94e49ce7 (ECG to detect atrial fibrillation and other acute arrhythmias)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>activity1 (Rapid initial evaluation for airway, breathing, and circulation)</t>
+          <t>id512023c8-f0a8-48a8-9725-fd4ec6f2e87b (Parallel Gateway)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>parallelgateway1 (Parallel Gateway)</t>
+          <t>idf3f98844-5585-448e-babc-70a945e4d10e (Exclusive Gateway)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>dummy_Flow_2 ((dummy branch entry))</t>
+          <t>idb3e42d2d-0545-4d8b-8a72-d0a387b6638e (Immediate brain imaging (CT or MRI))</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>activity2-1 (neurological examination to determine focal neurological deficits and assess stroke severity on a standardized stroke scale (NIHSS or CNS for stroke))</t>
+          <t>id086edce5-0f2f-478b-998e-f9a4917dca6d (Upon EMS prenotification, contact and call acute stroke team to ED)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>activity2-2 (neurological examination to determine focal neurological deficits and assess stroke severity on a standardized stroke scale (NIHSS or CNS for stroke))</t>
+          <t>id1a8d4a8f-ec1a-4433-b8c9-64e2212aa41b (CTAS I/II access to diagnostic imaging for suspected stroke/TIA patients)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>dummy_Flow_5 ((dummy branch entry))</t>
+          <t>id5c3d8696-c258-4943-9d1d-e42399ba9641 (start)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>activity3-1 (Immediate brain imaging (CT or MRI))</t>
+          <t>id9b4b6cf6-2352-4b6e-a108-1397198fdcf5 (Use a standard triage tool to determine the appropriate location for the care of patients
+(Patients with TIA))</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>activity3-2 (Immediate brain imaging (CT or MRI))</t>
+          <t>id17335463-839f-4891-80ab-3c9d83796173 (Monitor patient closely and swallowing ability screened when clinically appropriate)</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>activity4 (Immediate expert healthcare provider interpretation of the brain imaging)</t>
+          <t>iddc7e020c-19ec-45db-a673-a4125e13bbb7 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>activity5 (ECG to detect atrial fibrillation and other acute arrhythmias)</t>
+          <t>idba97da51-dd94-4a7e-ac8d-980043a5c814 (Exclusive Merge)</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>activity6 (Chest x-ray without delay for for thrombolysis assessment)</t>
+          <t>idc4acaf5c-3b0f-41bb-b735-ff31c28b4fb8 (Exclusive Merge)</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>dummy_Flow_9 ((dummy branch entry))</t>
+          <t>id1cd19994-2445-4155-a2b8-65bb2823abd0 (Rapid initial evaluation for airway, breathing, and circulation)</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>activity7-1 (Blood work: CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
+          <t>id7961c11c-d68e-4ab5-aae2-a2caf4cac86a (Vascular imaging of the brain and neck arteries ASAP)</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>activity7-2 (Blood work: CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
+          <t>idcec5f945-9a53-407f-89b7-c2e800cc6270 (Blood work:
+ CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>dummy_Flow_12 ((dummy branch entry))</t>
+          <t>id22f118f9-464b-48f5-9953-411173ea0ff7 (Referral process for rapid-assessment TIA/minor stroke units or clinics for non-admitted patients)</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>activity8 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
+          <t>id0be010cc-37c2-424b-af57-b626019f3e62 (Full clinical assessment of the patient's swallowing ability by an expert (by a speech-language pathologist or appropriately trained specialist who would advise on swallowing ability and the required consistency of diet and fluids))</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>exclusivegateway1 (Exclusive Gateway)</t>
+          <t>id74c1daa1-959b-4d5d-9108-b958453f20ea (Immediate expert healthcare provider interpretation of the brain imaging)</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>activity9 (Monitor patient closely and swallowing ability screened when clinically appropriate)</t>
+          <t>id3b706ccd-c4ac-415a-9853-e6e5ca45a80d (end)</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>activity10 (Full clinical assessment of the patient's swallowing ability by an expert (by a speech-language pathologist or appropriately trained specialist who would advise on swallowing ability and the required consistency of diet and fluids))</t>
+          <t>ida9c8ae78-d909-4799-822f-50f9a5169da6 (EMS prenotifies receiving hospital about stroke/TIA patient arrival)</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>exclusivegateway1Join (Exclusive Merge)</t>
+          <t>idbc6300db-2ab5-4847-b297-6823f22c5b82 (Exclusive Merge)</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>activity11 (Give patients appropriate cross-continuum secondary prevention assessments and therapies (All patients, whether admitted or discharged from the ED))</t>
+          <t>id153ef512-56cb-470e-9153-70f33876ec49 (neurological examination to determine focal neurological deficits and assess stroke severity on a standardized stroke scale (NIHSS or CNS for stroke))</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>activity12 (Use a standard triage tool to determine the appropriate location for the care of patients (Patients with TIA))</t>
+          <t>id8438b44b-7538-4817-bdcc-17b94b90b7b5 (EMS diverts suspected stroke/TIA patients to regional/district stroke centres (where feasible))</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>exclusivegateway2 (Exclusive Gateway)</t>
+          <t>id7f070bdf-5d17-44da-85b4-935f3e2d389d (Give patients appropriate cross-continuum secondary prevention assessments and therapies
+(All patients, whether admitted or discharged from the ED)</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>activity13 (Immediate vascular imaging of the neck arteries (carotid ultrasound, CTA, or MRA))</t>
+          <t>idb19c2016-a92c-4df8-a139-df196c97b9be (Exclusive Gateway)</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>activity14 (Vascular imaging of the brain and neck arteries ASAP)</t>
+          <t>idba6b110b-3f93-48bf-977b-29ede8089823 (Exclusive Gateway)</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>exclusivegateway2Join (Exclusive Merge)</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>parallelgateway1Join (Parallel Merge)</t>
+          <t>ida6d1e95a-443e-40bb-9043-de93794ea1f2 (Parallel Merge)</t>
         </is>
       </c>
     </row>
@@ -587,7 +585,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -608,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -668,9 +666,6 @@
         <v>0</v>
       </c>
       <c r="AC2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -681,90 +676,87 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.1975308641975309</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.1746031746031746</v>
       </c>
       <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.253968253968254</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.196969696969697</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.1805555555555556</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.2477064220183486</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.2409638554216867</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.2209302325581395</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.1746031746031746</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="P3" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.2268041237113402</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.1861471861471862</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.2361111111111112</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.1791044776119403</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
         <v>0.214765100671141</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.214765100671141</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.1746031746031746</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.253968253968254</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.253968253968254</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.2361111111111112</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.1746031746031746</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.1746031746031746</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.1746031746031746</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.2325581395348837</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.2325581395348837</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.1746031746031746</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0.2209302325581395</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0.2409638554216867</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.1861471861471862</v>
-      </c>
-      <c r="W3" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" t="n">
-        <v>0.1972789115646258</v>
-      </c>
       <c r="Y3" t="n">
-        <v>0.2568807339449541</v>
+        <v>0.223404255319149</v>
       </c>
       <c r="Z3" t="n">
-        <v>0</v>
+        <v>0.1986301369863014</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.1975308641975309</v>
+        <v>0</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.2380952380952381</v>
+        <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -775,90 +767,87 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.2348993288590604</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.2348993288590604</v>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.1476510067114094</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.2281879194630873</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.2281879194630873</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.2885906040268457</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.2416107382550335</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.2325581395348837</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
         <v>0.214765100671141</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.09395973154362414</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="P4" t="n">
+        <v>0.2013422818791947</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.174496644295302</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.2281879194630873</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.2683982683982684</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.2080536912751678</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.2214765100671141</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
         <v>1</v>
       </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.09395973154362414</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.1476510067114094</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1476510067114094</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.2080536912751678</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.2348993288590604</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.1879194630872483</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.09395973154362414</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.1812080536912751</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.1812080536912751</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.09395973154362414</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.2325581395348837</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.2416107382550335</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0.2683982683982684</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0.1812080536912751</v>
-      </c>
       <c r="Y4" t="n">
-        <v>0.2953020134228188</v>
+        <v>0.2684563758389261</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
+        <v>0.174496644295302</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.2348993288590604</v>
+        <v>0</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.2013422818791947</v>
+        <v>0</v>
       </c>
       <c r="AC4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -869,90 +858,87 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.3580246913580247</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.2295081967213115</v>
       </c>
       <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.1743119266055045</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.1686746987951807</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.1279069767441861</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
         <v>0.253968253968254</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.2571428571428571</v>
-      </c>
-      <c r="G5" t="n">
+      <c r="P5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.1649484536082474</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.09956709956709953</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.3055555555555556</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.1940298507462687</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
         <v>0.1476510067114094</v>
       </c>
-      <c r="H5" t="n">
-        <v>0.1476510067114094</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.2571428571428571</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.3055555555555556</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.2295081967213115</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.2571428571428571</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.1550387596899225</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.1550387596899225</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.2571428571428571</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.1279069767441861</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.1686746987951807</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.09956709956709953</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0.1428571428571429</v>
-      </c>
       <c r="Y5" t="n">
-        <v>0.1743119266055045</v>
+        <v>0.1914893617021277</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>0.136986301369863</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.3580246913580247</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -963,90 +949,87 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.2592592592592593</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.2638888888888888</v>
       </c>
       <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.3055555555555556</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1805555555555556</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.1388888888888888</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.3027522935779816</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.1807228915662651</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.2209302325581395</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
         <v>0.2361111111111112</v>
       </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.1388888888888888</v>
-      </c>
-      <c r="G6" t="n">
+      <c r="P6" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.2371134020618557</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.2034632034632035</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.1666666666666666</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
         <v>0.2080536912751678</v>
       </c>
-      <c r="H6" t="n">
-        <v>0.2080536912751678</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.1388888888888888</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.3055555555555556</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.3055555555555556</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.2638888888888888</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.1388888888888888</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.2325581395348837</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.2325581395348837</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.1388888888888888</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.2209302325581395</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.1807228915662651</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0.2034632034632035</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0.2721088435374149</v>
-      </c>
       <c r="Y6" t="n">
-        <v>0.3119266055045872</v>
+        <v>0.2659574468085106</v>
       </c>
       <c r="Z6" t="n">
-        <v>0</v>
+        <v>0.273972602739726</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.2592592592592593</v>
+        <v>0</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.2222222222222222</v>
+        <v>0</v>
       </c>
       <c r="AC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1057,90 +1040,87 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.1975308641975309</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.2295081967213115</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.2575757575757576</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.2752293577981652</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.2771084337349398</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.1976744186046512</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
         <v>0.1746031746031746</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.180327868852459</v>
-      </c>
-      <c r="G7" t="n">
+      <c r="P7" t="n">
+        <v>0.2459016393442623</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.2384615384615385</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.2061855670103093</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.1688311688311688</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.2638888888888888</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.2089552238805971</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
         <v>0.2348993288590604</v>
       </c>
-      <c r="H7" t="n">
-        <v>0.2348993288590604</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.180327868852459</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.2295081967213115</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.2295081967213115</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.2638888888888888</v>
-      </c>
-      <c r="M7" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.180327868852459</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.180327868852459</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.248062015503876</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.248062015503876</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0.180327868852459</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.1976744186046512</v>
-      </c>
-      <c r="T7" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" t="n">
-        <v>0.2771084337349398</v>
-      </c>
-      <c r="V7" t="n">
-        <v>0.1688311688311688</v>
-      </c>
-      <c r="W7" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" t="n">
-        <v>0.2380952380952381</v>
-      </c>
       <c r="Y7" t="n">
-        <v>0.2844036697247706</v>
+        <v>0.2553191489361702</v>
       </c>
       <c r="Z7" t="n">
-        <v>0</v>
+        <v>0.2397260273972602</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.1975308641975309</v>
+        <v>0</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.2459016393442623</v>
+        <v>0</v>
       </c>
       <c r="AC7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1151,13 +1131,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.1975308641975309</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.180327868852459</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1746031746031746</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -1166,75 +1146,72 @@
         <v>0.1403508771929824</v>
       </c>
       <c r="G8" t="n">
+        <v>0.1515151515151515</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.2083333333333334</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.2568807339449541</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.2168674698795181</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.2034883720930233</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.1746031746031746</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.1403508771929824</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.2230769230769231</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.2371134020618557</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.1558441558441559</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.1492537313432836</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
         <v>0.1879194630872483</v>
       </c>
-      <c r="H8" t="n">
-        <v>0.1879194630872483</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.180327868852459</v>
-      </c>
-      <c r="N8" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.2248062015503876</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.2248062015503876</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0.2034883720930233</v>
-      </c>
-      <c r="T8" t="n">
-        <v>0</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0.2168674698795181</v>
-      </c>
-      <c r="V8" t="n">
-        <v>0.1558441558441559</v>
-      </c>
-      <c r="W8" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" t="n">
-        <v>0.1972789115646258</v>
-      </c>
       <c r="Y8" t="n">
-        <v>0.2660550458715596</v>
+        <v>0.2021276595744681</v>
       </c>
       <c r="Z8" t="n">
-        <v>0</v>
+        <v>0.1917808219178082</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.1975308641975309</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.1403508771929824</v>
+        <v>0</v>
       </c>
       <c r="AC8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1246,90 +1223,87 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.2076923076923077</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.2384615384615385</v>
       </c>
       <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.2307692307692307</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.1153846153846154</v>
-      </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
+        <v>0.2076923076923077</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.2461538461538462</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.2769230769230769</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.2441860465116279</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.1923076923076923</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.2076923076923077</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.2251082251082251</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.2615384615384615</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
         <v>0.174496644295302</v>
       </c>
-      <c r="H9" t="n">
-        <v>0.174496644295302</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.1153846153846154</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.1538461538461539</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.1538461538461539</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.2307692307692307</v>
-      </c>
-      <c r="M9" t="n">
+      <c r="Y9" t="n">
         <v>0.2384615384615385</v>
       </c>
-      <c r="N9" t="n">
-        <v>0.2230769230769231</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.1153846153846154</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.9846153846153847</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.9846153846153847</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0.1153846153846154</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.2441860465116279</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0.2769230769230769</v>
-      </c>
-      <c r="V9" t="n">
-        <v>0.2251082251082251</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" t="n">
-        <v>0.1904761904761905</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>0.2538461538461538</v>
-      </c>
       <c r="Z9" t="n">
-        <v>0</v>
+        <v>0.178082191780822</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.2076923076923077</v>
+        <v>0</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.1923076923076923</v>
+        <v>0</v>
       </c>
       <c r="AC9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1340,90 +1314,87 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.2441860465116279</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.1976744186046512</v>
       </c>
       <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.1279069767441861</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.2093023255813954</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.1918604651162791</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.2558139534883721</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.2906976744186046</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
         <v>0.2209302325581395</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.07558139534883723</v>
-      </c>
-      <c r="G10" t="n">
+      <c r="P10" t="n">
+        <v>0.1918604651162791</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.2441860465116279</v>
+      </c>
+      <c r="R10" t="n">
         <v>0.2325581395348837</v>
       </c>
-      <c r="H10" t="n">
+      <c r="S10" t="n">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.2209302325581395</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.2151162790697675</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" t="n">
         <v>0.2325581395348837</v>
       </c>
-      <c r="I10" t="n">
-        <v>0.07558139534883723</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.1279069767441861</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.1279069767441861</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.2209302325581395</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.1976744186046512</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.2034883720930233</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.07558139534883723</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0.07558139534883723</v>
-      </c>
-      <c r="S10" t="n">
-        <v>1</v>
-      </c>
-      <c r="T10" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0.2906976744186046</v>
-      </c>
-      <c r="V10" t="n">
-        <v>0.2727272727272727</v>
-      </c>
-      <c r="W10" t="n">
-        <v>0</v>
-      </c>
-      <c r="X10" t="n">
+      <c r="Y10" t="n">
+        <v>0.2093023255813954</v>
+      </c>
+      <c r="Z10" t="n">
         <v>0.2674418604651163</v>
       </c>
-      <c r="Y10" t="n">
-        <v>0.2616279069767442</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>0</v>
-      </c>
       <c r="AA10" t="n">
-        <v>0.2441860465116279</v>
+        <v>0</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.1918604651162791</v>
+        <v>0</v>
       </c>
       <c r="AC10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1434,90 +1405,87 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.1325301204819277</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.2771084337349398</v>
       </c>
       <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1686746987951807</v>
+      </c>
+      <c r="G11" t="n">
         <v>0.2409638554216867</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.1084337349397591</v>
-      </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
+        <v>0.1927710843373494</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.2110091743119266</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.2906976744186046</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.2409638554216867</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.2168674698795181</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.2769230769230769</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.2371134020618557</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.1807228915662651</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.2530120481927711</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
         <v>0.2416107382550335</v>
       </c>
-      <c r="H11" t="n">
-        <v>0.2416107382550335</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.1084337349397591</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.1686746987951807</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.1686746987951807</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.1807228915662651</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.2771084337349398</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.2168674698795181</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.1084337349397591</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.2790697674418605</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0.2790697674418605</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0.1084337349397591</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0.2906976744186046</v>
-      </c>
-      <c r="T11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U11" t="n">
-        <v>1</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0.2380952380952381</v>
-      </c>
-      <c r="W11" t="n">
-        <v>0</v>
-      </c>
-      <c r="X11" t="n">
-        <v>0.2312925170068028</v>
-      </c>
       <c r="Y11" t="n">
-        <v>0.2110091743119266</v>
+        <v>0.2127659574468085</v>
       </c>
       <c r="Z11" t="n">
-        <v>0</v>
+        <v>0.2328767123287672</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.1325301204819277</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.2168674698795181</v>
+        <v>0</v>
       </c>
       <c r="AC11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1528,90 +1496,87 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.1688311688311688</v>
       </c>
       <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.09956709956709953</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1731601731601732</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.1731601731601732</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.2510822510822511</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
         <v>0.1861471861471862</v>
       </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.06926406926406925</v>
-      </c>
-      <c r="G12" t="n">
+      <c r="P12" t="n">
+        <v>0.1471861471861472</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.2251082251082251</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.2077922077922078</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.2034632034632035</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.1731601731601732</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
         <v>0.2683982683982684</v>
       </c>
-      <c r="H12" t="n">
-        <v>0.2683982683982684</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.06926406926406925</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.09956709956709953</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.09956709956709953</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.2034632034632035</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.1688311688311688</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.1558441558441559</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0.06926406926406925</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.2294372294372294</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0.2294372294372294</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0.06926406926406925</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0.2727272727272727</v>
-      </c>
-      <c r="T12" t="n">
-        <v>0</v>
-      </c>
-      <c r="U12" t="n">
-        <v>0.2380952380952381</v>
-      </c>
-      <c r="V12" t="n">
-        <v>1</v>
-      </c>
-      <c r="W12" t="n">
-        <v>0</v>
-      </c>
-      <c r="X12" t="n">
-        <v>0.2597402597402597</v>
-      </c>
       <c r="Y12" t="n">
-        <v>0.2554112554112554</v>
+        <v>0.1991341991341992</v>
       </c>
       <c r="Z12" t="n">
-        <v>0</v>
+        <v>0.2510822510822511</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.1818181818181818</v>
+        <v>0</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.1471861471861472</v>
+        <v>0</v>
       </c>
       <c r="AC12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1705,9 +1670,6 @@
       <c r="AC13" t="n">
         <v>0</v>
       </c>
-      <c r="AD13" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1717,90 +1679,87 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>0.2534246575342466</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>0.2397260273972602</v>
       </c>
       <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.136986301369863</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.2671232876712328</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.2123287671232876</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.2671232876712328</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.2328767123287672</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.2674418604651163</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
         <v>0.1986301369863014</v>
       </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.08904109589041098</v>
-      </c>
-      <c r="G14" t="n">
+      <c r="P14" t="n">
+        <v>0.1986301369863014</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.178082191780822</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.2808219178082192</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.2510822510822511</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.273972602739726</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.2465753424657534</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" t="n">
         <v>0.174496644295302</v>
       </c>
-      <c r="H14" t="n">
-        <v>0.174496644295302</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.08904109589041098</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.136986301369863</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.136986301369863</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.273972602739726</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.2397260273972602</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.1917808219178082</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0.08904109589041098</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0.184931506849315</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0.184931506849315</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0.08904109589041098</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0.2674418604651163</v>
-      </c>
-      <c r="T14" t="n">
-        <v>0</v>
-      </c>
-      <c r="U14" t="n">
-        <v>0.2328767123287672</v>
-      </c>
-      <c r="V14" t="n">
-        <v>0.2510822510822511</v>
-      </c>
-      <c r="W14" t="n">
-        <v>0</v>
-      </c>
-      <c r="X14" t="n">
-        <v>0.9863945578231292</v>
-      </c>
       <c r="Y14" t="n">
-        <v>0.273972602739726</v>
+        <v>0.2602739726027398</v>
       </c>
       <c r="Z14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.2534246575342466</v>
+        <v>0</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.1986301369863014</v>
+        <v>0</v>
       </c>
       <c r="AC14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1812,90 +1771,87 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>0.2385321100917431</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>0.2752293577981652</v>
       </c>
       <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.1743119266055045</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.2385321100917431</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.2660550458715596</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.2110091743119266</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.2558139534883721</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
         <v>0.2477064220183486</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.1100917431192661</v>
-      </c>
-      <c r="G15" t="n">
+      <c r="P15" t="n">
+        <v>0.2752293577981652</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.2461538461538462</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.2110091743119266</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.2510822510822511</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.3027522935779816</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.2752293577981652</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" t="n">
         <v>0.2885906040268457</v>
       </c>
-      <c r="H15" t="n">
-        <v>0.2885906040268457</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.1100917431192661</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.1743119266055045</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.1743119266055045</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.3027522935779816</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.2752293577981652</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0.2568807339449541</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0.1100917431192661</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0.2403100775193798</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>0.2403100775193798</v>
-      </c>
-      <c r="R15" t="n">
-        <v>0.1100917431192661</v>
-      </c>
-      <c r="S15" t="n">
-        <v>0.2558139534883721</v>
-      </c>
-      <c r="T15" t="n">
-        <v>0</v>
-      </c>
-      <c r="U15" t="n">
+      <c r="Y15" t="n">
         <v>0.2110091743119266</v>
       </c>
-      <c r="V15" t="n">
-        <v>0.2510822510822511</v>
-      </c>
-      <c r="W15" t="n">
-        <v>0</v>
-      </c>
-      <c r="X15" t="n">
-        <v>0.2789115646258503</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>0.9908256880733946</v>
-      </c>
       <c r="Z15" t="n">
-        <v>0</v>
+        <v>0.2671232876712328</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.2385321100917431</v>
+        <v>0</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.2752293577981652</v>
+        <v>0</v>
       </c>
       <c r="AC15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1915,7 +1871,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -1939,10 +1895,10 @@
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="O16" t="n">
         <v>0</v>
@@ -1960,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
@@ -1978,18 +1934,15 @@
         <v>0</v>
       </c>
       <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
         <v>1</v>
       </c>
-      <c r="AA16" t="n">
-        <v>0</v>
-      </c>
       <c r="AB16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.6470588235294117</v>
-      </c>
-      <c r="AD16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2000,90 +1953,87 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>0.1975308641975309</v>
       </c>
       <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3580246913580247</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.2345679012345679</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.2098765432098766</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.2385321100917431</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.1325301204819277</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.2441860465116279</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
         <v>0.1975308641975309</v>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.1358024691358025</v>
-      </c>
-      <c r="G17" t="n">
+      <c r="P17" t="n">
+        <v>0.3950617283950617</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.2076923076923077</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.1958762886597938</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.2592592592592593</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.1728395061728395</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" t="n">
         <v>0.2348993288590604</v>
       </c>
-      <c r="H17" t="n">
-        <v>0.2348993288590604</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.1358024691358025</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.3580246913580247</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.3580246913580247</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.2592592592592593</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.1975308641975309</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0.1975308641975309</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0.1358024691358025</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0.2093023255813954</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0.2093023255813954</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0.1358024691358025</v>
-      </c>
-      <c r="S17" t="n">
-        <v>0.2441860465116279</v>
-      </c>
-      <c r="T17" t="n">
-        <v>0</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.1325301204819277</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0.1818181818181818</v>
-      </c>
-      <c r="W17" t="n">
-        <v>0</v>
-      </c>
-      <c r="X17" t="n">
-        <v>0.2653061224489796</v>
-      </c>
       <c r="Y17" t="n">
-        <v>0.2477064220183486</v>
+        <v>0.2127659574468085</v>
       </c>
       <c r="Z17" t="n">
-        <v>0</v>
+        <v>0.2534246575342466</v>
       </c>
       <c r="AA17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.3950617283950617</v>
+        <v>0</v>
       </c>
       <c r="AC17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2094,90 +2044,87 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>0.3950617283950617</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>0.2459016393442623</v>
       </c>
       <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.2424242424242424</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.2361111111111112</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.2752293577981652</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.2168674698795181</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.1918604651162791</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
         <v>0.2380952380952381</v>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.2115384615384616</v>
-      </c>
-      <c r="G18" t="n">
+      <c r="P18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.1923076923076923</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.2164948453608248</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.1471861471861472</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.1940298507462687</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" t="n">
         <v>0.2013422818791947</v>
       </c>
-      <c r="H18" t="n">
-        <v>0.2013422818791947</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.2115384615384616</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0.2459016393442623</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0.2115384615384616</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0.1937984496124031</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0.1937984496124031</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0.2115384615384616</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0.1918604651162791</v>
-      </c>
-      <c r="T18" t="n">
-        <v>0</v>
-      </c>
-      <c r="U18" t="n">
-        <v>0.2168674698795181</v>
-      </c>
-      <c r="V18" t="n">
-        <v>0.1471861471861472</v>
-      </c>
-      <c r="W18" t="n">
-        <v>0</v>
-      </c>
-      <c r="X18" t="n">
-        <v>0.1972789115646258</v>
-      </c>
       <c r="Y18" t="n">
-        <v>0.2752293577981652</v>
+        <v>0.2127659574468085</v>
       </c>
       <c r="Z18" t="n">
-        <v>0</v>
+        <v>0.1986301369863014</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.3950617283950617</v>
+        <v>0</v>
       </c>
       <c r="AB18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2197,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -2221,10 +2168,10 @@
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" t="n">
         <v>0</v>
@@ -2242,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>0.6470588235294117</v>
+        <v>0</v>
       </c>
       <c r="U19" t="n">
         <v>0</v>
@@ -2260,18 +2207,15 @@
         <v>0</v>
       </c>
       <c r="Z19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="AA19" t="n">
-        <v>0</v>
-      </c>
       <c r="AB19" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="AC19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2285,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -2339,7 +2283,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="n">
-        <v>0</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="V20" t="n">
         <v>0</v>
@@ -2363,9 +2307,6 @@
         <v>0</v>
       </c>
       <c r="AC20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2382,10 +2323,10 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -2457,9 +2398,6 @@
         <v>0</v>
       </c>
       <c r="AC21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD21" t="n">
         <v>0.625</v>
       </c>
     </row>
@@ -2553,9 +2491,6 @@
       <c r="AC22" t="n">
         <v>0</v>
       </c>
-      <c r="AD22" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -2573,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -2597,10 +2532,10 @@
         <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
@@ -2618,7 +2553,7 @@
         <v>0</v>
       </c>
       <c r="T23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" t="n">
         <v>0</v>
@@ -2636,18 +2571,15 @@
         <v>0</v>
       </c>
       <c r="Z23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="n">
         <v>1</v>
       </c>
-      <c r="AA23" t="n">
-        <v>0</v>
-      </c>
       <c r="AB23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.6470588235294117</v>
-      </c>
-      <c r="AD23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2667,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -2691,10 +2623,10 @@
         <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" t="n">
         <v>0</v>
@@ -2712,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="T24" t="n">
-        <v>0.6470588235294117</v>
+        <v>0</v>
       </c>
       <c r="U24" t="n">
         <v>0</v>
@@ -2730,18 +2662,15 @@
         <v>0</v>
       </c>
       <c r="Z24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="AA24" t="n">
-        <v>0</v>
-      </c>
       <c r="AB24" t="n">
-        <v>0</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="AC24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2758,10 +2687,10 @@
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="E25" t="n">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -2833,9 +2762,6 @@
         <v>0</v>
       </c>
       <c r="AC25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD25" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change layout_path; update INSTALL
</commit_message>
<xml_diff>
--- a/similarity_matrix.xlsx
+++ b/similarity_matrix.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,104 +451,109 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>parallelgateway1 (Parallel Gateway)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>activity2 (neurological examination to determine focal neurological deficits and assess stroke severity on a standardized stroke scale (NIHSS or CNS for stroke))</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>activity3 (Immediate brain imaging (CT or MRI))</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>activity4 (Immediate brain imaging (CT or MRI))</t>
+          <t>activity3-1 (Immediate brain imaging (CT or MRI))</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>parallelgateway1 (Parallel Gateway)</t>
+          <t>activity3-2 (Immediate brain imaging (CT or MRI))</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>activity5 (Immediate expert healthcare provider interpretation of the brain imaging)</t>
+          <t>activity4 (Immediate expert healthcare provider interpretation of the brain imaging)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>activity6 (ECG to detect atrial fibrillation and other acute arrhythmias)</t>
+          <t>activity5 (ECG to detect atrial fibrillation and other acute arrhythmias)</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>activity7_merged (Blood work:
+          <t>activity6 (Chest x-ray without delay for for thrombolysis assessment)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>activity7 (Blood work:
  CBC, electrolytes, creatinine, glucose, INR, partial thromboplastin time, and troponin test (if clinically indicated))</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>activity8 (Chest x-ray without delay for for thrombolysis assessment)</t>
-        </is>
-      </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>activity9 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
+          <t>activity9-1 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>activity9-2 (Make patient NPO (nothing by mouth) initially and screen their swallowing ability as part of their initial assessment and before initiating oral medication, fluid, or food.)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>exclusivegateway1 (Exclusive Gateway)</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>activity10 (Monitor patient closely and swallowing ability screened when clinically appropriate)</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>activity11 (Full clinical assessment of the patient's swallowing ability by an expert (by a speech-language pathologist or appropriately trained specialist who would advise on swallowing ability and the required consistency of diet and fluids))</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>exclusivegateway1Join (Exclusive Merge)</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>activity13 (Use a standard triage tool to determine the appropriate location for the care of patients
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>activity12 (Use a standard triage tool to determine the appropriate location for the care of patients
 (Patients with TIA))</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>exclusivegateway2 (Exclusive Gateway)</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>activity14 (Immediate vascular imaging of the neck arteries (carotid ultrasound, CTA, or MRA))</t>
-        </is>
-      </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>activity15 (Vascular imaging of the brain and neck arteries ASAP)</t>
+          <t>activity13 (Immediate vascular imaging of the neck arteries (carotid ultrasound, CTA, or MRA))</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
+          <t>activity14 (Vascular imaging of the brain and neck arteries ASAP)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
           <t>exclusivegateway2Join (Exclusive Merge)</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>parallelgateway1Join (Parallel Merge)</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>activity12 (Give patients appropriate cross-continuum secondary prevention assessments and therapies
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>activity15 (Give patients appropriate cross-continuum secondary prevention assessments and therapies
 (All patients, whether admitted or discharged from the ED)</t>
         </is>
       </c>
@@ -628,6 +633,9 @@
       <c r="X2" t="n">
         <v>0</v>
       </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -645,16 +653,16 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.214765100671141</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.253968253968254</v>
       </c>
       <c r="G3" t="n">
         <v>0.253968253968254</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.253968253968254</v>
       </c>
       <c r="I3" t="n">
         <v>0.2361111111111112</v>
@@ -663,45 +671,48 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="K3" t="n">
+        <v>0.1746031746031746</v>
+      </c>
+      <c r="L3" t="n">
         <v>0.2307692307692307</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.1746031746031746</v>
       </c>
       <c r="M3" t="n">
         <v>0.2209302325581395</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>0.2209302325581395</v>
       </c>
       <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
         <v>0.2409638554216867</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.1861471861471862</v>
       </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
       <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
         <v>0.2477064220183486</v>
       </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
       <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
         <v>0.1975308641975309</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.2380952380952381</v>
       </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
       <c r="W3" t="n">
         <v>0</v>
       </c>
       <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
         <v>0.1986301369863014</v>
       </c>
     </row>
@@ -721,16 +732,16 @@
         <v>0.214765100671141</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1476510067114094</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
         <v>0.1476510067114094</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.1476510067114094</v>
       </c>
       <c r="I4" t="n">
         <v>0.2080536912751678</v>
@@ -739,45 +750,48 @@
         <v>0.2348993288590604</v>
       </c>
       <c r="K4" t="n">
+        <v>0.1879194630872483</v>
+      </c>
+      <c r="L4" t="n">
         <v>0.174496644295302</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.1879194630872483</v>
       </c>
       <c r="M4" t="n">
         <v>0.2325581395348837</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>0.2325581395348837</v>
       </c>
       <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.2416107382550335</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>0.2683982683982684</v>
       </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
       <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
         <v>0.2885906040268457</v>
       </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
       <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
         <v>0.2348993288590604</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>0.2013422818791947</v>
       </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
       <c r="W4" t="n">
         <v>0</v>
       </c>
       <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
         <v>0.174496644295302</v>
       </c>
     </row>
@@ -797,16 +811,16 @@
         <v>0.253968253968254</v>
       </c>
       <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
         <v>0.1476510067114094</v>
       </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
       <c r="G5" t="n">
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
         <v>0.3055555555555556</v>
@@ -815,45 +829,48 @@
         <v>0.2295081967213115</v>
       </c>
       <c r="K5" t="n">
+        <v>0.1403508771929824</v>
+      </c>
+      <c r="L5" t="n">
         <v>0.1538461538461539</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.1403508771929824</v>
       </c>
       <c r="M5" t="n">
         <v>0.1279069767441861</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>0.1279069767441861</v>
       </c>
       <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
         <v>0.1686746987951807</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>0.09956709956709953</v>
       </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
       <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
         <v>0.1743119266055045</v>
       </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
       <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
         <v>0.3580246913580247</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>0.25</v>
       </c>
-      <c r="V5" t="n">
-        <v>0</v>
-      </c>
       <c r="W5" t="n">
         <v>0</v>
       </c>
       <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
         <v>0.136986301369863</v>
       </c>
     </row>
@@ -873,16 +890,16 @@
         <v>0.2361111111111112</v>
       </c>
       <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
         <v>0.2080536912751678</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.3055555555555556</v>
       </c>
       <c r="G6" t="n">
         <v>0.3055555555555556</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.3055555555555556</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -891,45 +908,48 @@
         <v>0.2638888888888888</v>
       </c>
       <c r="K6" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="L6" t="n">
         <v>0.2307692307692307</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.2222222222222222</v>
       </c>
       <c r="M6" t="n">
         <v>0.2209302325581395</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>0.2209302325581395</v>
       </c>
       <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
         <v>0.1807228915662651</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>0.2034632034632035</v>
       </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
       <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
         <v>0.3027522935779816</v>
       </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
       <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
         <v>0.2592592592592593</v>
       </c>
-      <c r="U6" t="n">
+      <c r="V6" t="n">
         <v>0.2222222222222222</v>
       </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
       <c r="W6" t="n">
         <v>0</v>
       </c>
       <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
         <v>0.273972602739726</v>
       </c>
     </row>
@@ -949,16 +969,16 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
         <v>0.2348993288590604</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.2295081967213115</v>
       </c>
       <c r="G7" t="n">
         <v>0.2295081967213115</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>0.2295081967213115</v>
       </c>
       <c r="I7" t="n">
         <v>0.2638888888888888</v>
@@ -967,45 +987,48 @@
         <v>1</v>
       </c>
       <c r="K7" t="n">
+        <v>0.180327868852459</v>
+      </c>
+      <c r="L7" t="n">
         <v>0.2384615384615385</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.180327868852459</v>
       </c>
       <c r="M7" t="n">
         <v>0.1976744186046512</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>0.1976744186046512</v>
       </c>
       <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
         <v>0.2771084337349398</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>0.1688311688311688</v>
       </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
       <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
         <v>0.2752293577981652</v>
       </c>
-      <c r="S7" t="n">
-        <v>0</v>
-      </c>
       <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
         <v>0.1975308641975309</v>
       </c>
-      <c r="U7" t="n">
+      <c r="V7" t="n">
         <v>0.2459016393442623</v>
       </c>
-      <c r="V7" t="n">
-        <v>0</v>
-      </c>
       <c r="W7" t="n">
         <v>0</v>
       </c>
       <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
         <v>0.2397260273972602</v>
       </c>
     </row>
@@ -1025,16 +1048,16 @@
         <v>0.1746031746031746</v>
       </c>
       <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
         <v>0.1879194630872483</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1403508771929824</v>
       </c>
       <c r="G8" t="n">
         <v>0.1403508771929824</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>0.1403508771929824</v>
       </c>
       <c r="I8" t="n">
         <v>0.2222222222222222</v>
@@ -1043,45 +1066,48 @@
         <v>0.180327868852459</v>
       </c>
       <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
         <v>0.2230769230769231</v>
-      </c>
-      <c r="L8" t="n">
-        <v>1</v>
       </c>
       <c r="M8" t="n">
         <v>0.2034883720930233</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>0.2034883720930233</v>
       </c>
       <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
         <v>0.2168674698795181</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>0.1558441558441559</v>
       </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
       <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
         <v>0.2568807339449541</v>
       </c>
-      <c r="S8" t="n">
-        <v>0</v>
-      </c>
       <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
         <v>0.1975308641975309</v>
       </c>
-      <c r="U8" t="n">
+      <c r="V8" t="n">
         <v>0.1403508771929824</v>
       </c>
-      <c r="V8" t="n">
-        <v>0</v>
-      </c>
       <c r="W8" t="n">
         <v>0</v>
       </c>
       <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
         <v>0.1917808219178082</v>
       </c>
     </row>
@@ -1102,16 +1128,16 @@
         <v>0.2307692307692307</v>
       </c>
       <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
         <v>0.174496644295302</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.1538461538461539</v>
       </c>
       <c r="G9" t="n">
         <v>0.1538461538461539</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="I9" t="n">
         <v>0.2307692307692307</v>
@@ -1120,45 +1146,48 @@
         <v>0.2384615384615385</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>0.2230769230769231</v>
       </c>
       <c r="L9" t="n">
-        <v>0.2230769230769231</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
         <v>0.2441860465116279</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>0.2441860465116279</v>
       </c>
       <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
         <v>0.2769230769230769</v>
       </c>
-      <c r="P9" t="n">
+      <c r="Q9" t="n">
         <v>0.2251082251082251</v>
       </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
       <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
         <v>0.2461538461538462</v>
       </c>
-      <c r="S9" t="n">
-        <v>0</v>
-      </c>
       <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
         <v>0.2076923076923077</v>
       </c>
-      <c r="U9" t="n">
+      <c r="V9" t="n">
         <v>0.1923076923076923</v>
       </c>
-      <c r="V9" t="n">
-        <v>0</v>
-      </c>
       <c r="W9" t="n">
         <v>0</v>
       </c>
       <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
         <v>0.178082191780822</v>
       </c>
     </row>
@@ -1178,16 +1207,16 @@
         <v>0.2209302325581395</v>
       </c>
       <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0.2325581395348837</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.1279069767441861</v>
       </c>
       <c r="G10" t="n">
         <v>0.1279069767441861</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.1279069767441861</v>
       </c>
       <c r="I10" t="n">
         <v>0.2209302325581395</v>
@@ -1196,45 +1225,48 @@
         <v>0.1976744186046512</v>
       </c>
       <c r="K10" t="n">
+        <v>0.2034883720930233</v>
+      </c>
+      <c r="L10" t="n">
         <v>0.2441860465116279</v>
       </c>
-      <c r="L10" t="n">
-        <v>0.2034883720930233</v>
-      </c>
       <c r="M10" t="n">
         <v>1</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
         <v>0.2906976744186046</v>
       </c>
-      <c r="P10" t="n">
+      <c r="Q10" t="n">
         <v>0.2727272727272727</v>
       </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
       <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
         <v>0.2558139534883721</v>
       </c>
-      <c r="S10" t="n">
-        <v>0</v>
-      </c>
       <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
         <v>0.2441860465116279</v>
       </c>
-      <c r="U10" t="n">
+      <c r="V10" t="n">
         <v>0.1918604651162791</v>
       </c>
-      <c r="V10" t="n">
-        <v>0</v>
-      </c>
       <c r="W10" t="n">
         <v>0</v>
       </c>
       <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
         <v>0.2674418604651163</v>
       </c>
     </row>
@@ -1254,16 +1286,16 @@
         <v>0.2409638554216867</v>
       </c>
       <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
         <v>0.2416107382550335</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.1686746987951807</v>
       </c>
       <c r="G11" t="n">
         <v>0.1686746987951807</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.1686746987951807</v>
       </c>
       <c r="I11" t="n">
         <v>0.1807228915662651</v>
@@ -1272,45 +1304,48 @@
         <v>0.2771084337349398</v>
       </c>
       <c r="K11" t="n">
+        <v>0.2168674698795181</v>
+      </c>
+      <c r="L11" t="n">
         <v>0.2769230769230769</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.2168674698795181</v>
       </c>
       <c r="M11" t="n">
         <v>0.2906976744186046</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>0.2906976744186046</v>
       </c>
       <c r="O11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="n">
         <v>0.2380952380952381</v>
       </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
       <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
         <v>0.2110091743119266</v>
       </c>
-      <c r="S11" t="n">
-        <v>0</v>
-      </c>
       <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
         <v>0.1325301204819277</v>
       </c>
-      <c r="U11" t="n">
+      <c r="V11" t="n">
         <v>0.2168674698795181</v>
       </c>
-      <c r="V11" t="n">
-        <v>0</v>
-      </c>
       <c r="W11" t="n">
         <v>0</v>
       </c>
       <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
         <v>0.2328767123287672</v>
       </c>
     </row>
@@ -1330,16 +1365,16 @@
         <v>0.1861471861471862</v>
       </c>
       <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
         <v>0.2683982683982684</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.09956709956709953</v>
       </c>
       <c r="G12" t="n">
         <v>0.09956709956709953</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>0.09956709956709953</v>
       </c>
       <c r="I12" t="n">
         <v>0.2034632034632035</v>
@@ -1348,45 +1383,48 @@
         <v>0.1688311688311688</v>
       </c>
       <c r="K12" t="n">
+        <v>0.1558441558441559</v>
+      </c>
+      <c r="L12" t="n">
         <v>0.2251082251082251</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.1558441558441559</v>
       </c>
       <c r="M12" t="n">
         <v>0.2727272727272727</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
         <v>0.2380952380952381</v>
       </c>
-      <c r="P12" t="n">
-        <v>1</v>
-      </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
         <v>0.2510822510822511</v>
       </c>
-      <c r="S12" t="n">
-        <v>0</v>
-      </c>
       <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
         <v>0.1818181818181818</v>
       </c>
-      <c r="U12" t="n">
+      <c r="V12" t="n">
         <v>0.1471861471861472</v>
       </c>
-      <c r="V12" t="n">
-        <v>0</v>
-      </c>
       <c r="W12" t="n">
         <v>0</v>
       </c>
       <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="n">
         <v>0.2510822510822511</v>
       </c>
     </row>
@@ -1465,6 +1503,9 @@
       <c r="X13" t="n">
         <v>0</v>
       </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1483,16 +1524,16 @@
         <v>0.1986301369863014</v>
       </c>
       <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
         <v>0.174496644295302</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.136986301369863</v>
       </c>
       <c r="G14" t="n">
         <v>0.136986301369863</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>0.136986301369863</v>
       </c>
       <c r="I14" t="n">
         <v>0.273972602739726</v>
@@ -1501,45 +1542,48 @@
         <v>0.2397260273972602</v>
       </c>
       <c r="K14" t="n">
+        <v>0.1917808219178082</v>
+      </c>
+      <c r="L14" t="n">
         <v>0.178082191780822</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.1917808219178082</v>
       </c>
       <c r="M14" t="n">
         <v>0.2674418604651163</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>0.2674418604651163</v>
       </c>
       <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
         <v>0.2328767123287672</v>
       </c>
-      <c r="P14" t="n">
+      <c r="Q14" t="n">
         <v>0.2510822510822511</v>
       </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
       <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
         <v>0.2671232876712328</v>
       </c>
-      <c r="S14" t="n">
-        <v>0</v>
-      </c>
       <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
         <v>0.2534246575342466</v>
       </c>
-      <c r="U14" t="n">
+      <c r="V14" t="n">
         <v>0.1986301369863014</v>
       </c>
-      <c r="V14" t="n">
-        <v>0</v>
-      </c>
       <c r="W14" t="n">
         <v>0</v>
       </c>
       <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1560,16 +1604,16 @@
         <v>0.2477064220183486</v>
       </c>
       <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
         <v>0.2885906040268457</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.1743119266055045</v>
       </c>
       <c r="G15" t="n">
         <v>0.1743119266055045</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>0.1743119266055045</v>
       </c>
       <c r="I15" t="n">
         <v>0.3027522935779816</v>
@@ -1578,45 +1622,48 @@
         <v>0.2752293577981652</v>
       </c>
       <c r="K15" t="n">
+        <v>0.2568807339449541</v>
+      </c>
+      <c r="L15" t="n">
         <v>0.2461538461538462</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.2568807339449541</v>
       </c>
       <c r="M15" t="n">
         <v>0.2558139534883721</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>0.2558139534883721</v>
       </c>
       <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
         <v>0.2110091743119266</v>
       </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
         <v>0.2510822510822511</v>
       </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
       <c r="R15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
         <v>0.2385321100917431</v>
       </c>
-      <c r="U15" t="n">
+      <c r="V15" t="n">
         <v>0.2752293577981652</v>
       </c>
-      <c r="V15" t="n">
-        <v>0</v>
-      </c>
       <c r="W15" t="n">
         <v>0</v>
       </c>
       <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="n">
         <v>0.2671232876712328</v>
       </c>
     </row>
@@ -1663,36 +1710,39 @@
         <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="R16" t="n">
-        <v>0</v>
-      </c>
       <c r="S16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
       </c>
       <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="W16" t="n">
-        <v>0</v>
-      </c>
       <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1712,16 +1762,16 @@
         <v>0.1975308641975309</v>
       </c>
       <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
         <v>0.2348993288590604</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.3580246913580247</v>
       </c>
       <c r="G17" t="n">
         <v>0.3580246913580247</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>0.3580246913580247</v>
       </c>
       <c r="I17" t="n">
         <v>0.2592592592592593</v>
@@ -1730,45 +1780,48 @@
         <v>0.1975308641975309</v>
       </c>
       <c r="K17" t="n">
+        <v>0.1975308641975309</v>
+      </c>
+      <c r="L17" t="n">
         <v>0.2076923076923077</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.1975308641975309</v>
       </c>
       <c r="M17" t="n">
         <v>0.2441860465116279</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>0.2441860465116279</v>
       </c>
       <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
         <v>0.1325301204819277</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q17" t="n">
         <v>0.1818181818181818</v>
       </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
       <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
         <v>0.2385321100917431</v>
       </c>
-      <c r="S17" t="n">
-        <v>0</v>
-      </c>
       <c r="T17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17" t="n">
+        <v>1</v>
+      </c>
+      <c r="V17" t="n">
         <v>0.3950617283950617</v>
       </c>
-      <c r="V17" t="n">
-        <v>0</v>
-      </c>
       <c r="W17" t="n">
         <v>0</v>
       </c>
       <c r="X17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="n">
         <v>0.2534246575342466</v>
       </c>
     </row>
@@ -1788,16 +1841,16 @@
         <v>0.2380952380952381</v>
       </c>
       <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
         <v>0.2013422818791947</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.25</v>
       </c>
       <c r="G18" t="n">
         <v>0.25</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I18" t="n">
         <v>0.2222222222222222</v>
@@ -1806,45 +1859,48 @@
         <v>0.2459016393442623</v>
       </c>
       <c r="K18" t="n">
+        <v>0.1403508771929824</v>
+      </c>
+      <c r="L18" t="n">
         <v>0.1923076923076923</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.1403508771929824</v>
       </c>
       <c r="M18" t="n">
         <v>0.1918604651162791</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>0.1918604651162791</v>
       </c>
       <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
         <v>0.2168674698795181</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
         <v>0.1471861471861472</v>
       </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
       <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
         <v>0.2752293577981652</v>
       </c>
-      <c r="S18" t="n">
-        <v>0</v>
-      </c>
       <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
         <v>0.3950617283950617</v>
       </c>
-      <c r="U18" t="n">
-        <v>1</v>
-      </c>
       <c r="V18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" t="n">
         <v>0</v>
       </c>
       <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="n">
         <v>0.1986301369863014</v>
       </c>
     </row>
@@ -1891,36 +1947,39 @@
         <v>0</v>
       </c>
       <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
       <c r="P19" t="n">
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="T19" t="n">
-        <v>0</v>
-      </c>
       <c r="U19" t="n">
         <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1999,6 +2058,9 @@
       <c r="X20" t="n">
         <v>0</v>
       </c>
+      <c r="Y20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -2016,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -2025,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -2070,9 +2132,12 @@
         <v>0</v>
       </c>
       <c r="W21" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" t="n">
         <v>0.625</v>
       </c>
-      <c r="X21" t="n">
+      <c r="Y21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2151,6 +2216,9 @@
       <c r="X22" t="n">
         <v>0</v>
       </c>
+      <c r="Y22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -2195,36 +2263,39 @@
         <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23" t="n">
         <v>0</v>
       </c>
       <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="R23" t="n">
-        <v>0</v>
-      </c>
       <c r="S23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" t="n">
         <v>0</v>
       </c>
       <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="W23" t="n">
-        <v>0</v>
-      </c>
       <c r="X23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2271,36 +2342,39 @@
         <v>0</v>
       </c>
       <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
       <c r="P24" t="n">
         <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="T24" t="n">
-        <v>0</v>
-      </c>
       <c r="U24" t="n">
         <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2320,7 +2394,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -2329,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -2374,9 +2448,12 @@
         <v>0</v>
       </c>
       <c r="W25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X25" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y25" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>